<commit_message>
Updated pins connected to the SM
</commit_message>
<xml_diff>
--- a/Docs/CMv2_TM4C_controller_pin_specs.xlsx
+++ b/Docs/CMv2_TM4C_controller_pin_specs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\6089-119_CM_2xVU13P\GitHub\Cornell_CM_Rev2_HW\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18F9400B-9B80-4693-A41F-CF81545B5A3E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EC15CC8-9430-4C70-9B55-C56763B7D31E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="836" uniqueCount="485">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="831" uniqueCount="484">
   <si>
     <t>Pin Number</t>
   </si>
@@ -80,13 +80,7 @@
     <t>U0Rx</t>
   </si>
   <si>
-    <t>UART Module 0 receive</t>
-  </si>
-  <si>
     <t>U0Tx</t>
-  </si>
-  <si>
-    <t>UART Module 0 transmit</t>
   </si>
   <si>
     <t>Signal Name</t>
@@ -996,48 +990,24 @@
     <t>U3Tx</t>
   </si>
   <si>
-    <t>UART Module 3 receive</t>
-  </si>
-  <si>
-    <t>UART Module 3 transmit</t>
-  </si>
-  <si>
     <t>SM_IPMC_TX</t>
   </si>
   <si>
     <t>SM_IPMC_RX</t>
   </si>
   <si>
-    <t>UART for serial data transmitted from the IPMC module on the SM and received by the MCU</t>
-  </si>
-  <si>
-    <t>UART for serial data transmitted from the MCU and received by the IPMC module on the SM</t>
-  </si>
-  <si>
     <t>SM_ZYNQ_TX</t>
   </si>
   <si>
     <t>SM_ZYNQ_RX</t>
   </si>
   <si>
-    <t>UART for serial data transmitted from the ZYNQ module on the SM and received by the MCU</t>
-  </si>
-  <si>
-    <t>UART for serial data transmitted from the MCU and received by the ZYNQ module on the SM</t>
-  </si>
-  <si>
     <t>PA2</t>
   </si>
   <si>
     <t>PA3</t>
   </si>
   <si>
-    <t>GPIO port  A bit 2</t>
-  </si>
-  <si>
-    <t>GPIO port  A bit 3</t>
-  </si>
-  <si>
     <t>undef</t>
   </si>
   <si>
@@ -1056,12 +1026,6 @@
     <t>PA7</t>
   </si>
   <si>
-    <t>GPIO port  A bit 6</t>
-  </si>
-  <si>
-    <t>GPIO port  A bit 7</t>
-  </si>
-  <si>
     <t>SM_CPLD_GPIO1</t>
   </si>
   <si>
@@ -1071,37 +1035,7 @@
     <t>Connection to a GPIO pin on the CPLD on the SM (SMv2 or later). The use is currently undefined, but it can be used for I2C #6 SCL, UART #2 Rx, GPIO PA6, or Timer T3. This signal is tied to GND on the original SMv1. It initially has a 270 ohm resistor in series for current limiting.</t>
   </si>
   <si>
-    <t>Connection to a GPIO pin on the ZYNQ on the SM (SMv2 or later). The use is currently undefined, but it can be used for I2C #8 SCL, UART #4 Rx, GPIO PA2, or Timer T1. This signal is tied to GND on the original SMv1. It initially has a 270 ohm resistor in series for current limiting.</t>
-  </si>
-  <si>
-    <t>Connection to a GPIO pin on the ZYNQ on the SM (SMv2 or later). The use is currently undefined, but it can be used for I2C #8 SDA, UART #4 Tx, GPIO PA3, or Timer T1. This signal is tied to GND on the original SMv1. It initially has a 270 ohm resistor in series for current limiting.</t>
-  </si>
-  <si>
     <t>Connection to a GPIO pin on the CPLD on the SM (SMv2 or later). The use is currently undefined, but it can be used for I2C #6 SDA, UART #2 Tx, GPIO PA7, or timer T3. This signal is tied to GND on the original SMv1. It initially has a 270 ohm resistor in series for current limiting.</t>
-  </si>
-  <si>
-    <t>U7Tx</t>
-  </si>
-  <si>
-    <t>UART Module 7 transmit</t>
-  </si>
-  <si>
-    <t>MON_UART_TO_SM</t>
-  </si>
-  <si>
-    <t>GPIO port  C bit 4</t>
-  </si>
-  <si>
-    <t>SM_ZYNQ_GPIO0</t>
-  </si>
-  <si>
-    <t>Connection to a GPIO pin on the ZYNQ on the SM. The use is currently undefined, but it can be used for UART #7 Rx or GPIO PC4.</t>
-  </si>
-  <si>
-    <t>SM_MASTER_I2C_SDA</t>
-  </si>
-  <si>
-    <t>SM_MASTER_I2C_SCL</t>
   </si>
   <si>
     <t>FP_MCU_TDO</t>
@@ -1360,9 +1294,6 @@
   </si>
   <si>
     <t>2.10, 5.04, 6.04</t>
-  </si>
-  <si>
-    <t>2.03</t>
   </si>
   <si>
     <t>/F1_JTAG_BYPASS</t>
@@ -1425,9 +1356,6 @@
     <t>This output controls the write-protect pin on the ID EEPROM. Set this output LOW to enable writing to the EEPROM. Set this output HIGH to disable writing.</t>
   </si>
   <si>
-    <t>2.01</t>
-  </si>
-  <si>
     <t>This signal is used by the ZYNQ to tell the MCU to enable or disable power supplies on the CM. The ZYNQ will set it LOW to make the MCU disable all controllable power supplies. The ZYNQ will transition it to HIGH to start the MCU's power control state machine. There is not any pull-up on the CM, so configure it as an input with 2 mA internal pull-up to allow operation when not connected to the SM.</t>
   </si>
   <si>
@@ -1522,6 +1450,95 @@
   </si>
   <si>
     <t xml:space="preserve">Set this output HIGH to turn on the LT1764 power supply for FPGA#2's 1.8 volt V_F2_VCCAUX voltage. </t>
+  </si>
+  <si>
+    <t>SM_IPMC_I2C_SDA</t>
+  </si>
+  <si>
+    <t>SM_IPMC_I2C_SCL</t>
+  </si>
+  <si>
+    <t>SM_ZYNQ_I2C_SCL</t>
+  </si>
+  <si>
+    <t>SM_ZYNQ_I2C_SDA</t>
+  </si>
+  <si>
+    <t>Connection to a GPIO pin on the ZYNQ on the SM. The use is currently undefined, but it can be used for I2C #8 SCL, UART #4 Rx, GPIO PA2, or Timer T1.</t>
+  </si>
+  <si>
+    <t>Connection to a GPIO pin on the ZYNQ on the SM. The use is currently undefined, but it can be used for I2C #8 SDA, UART #4 Tx, GPIO PA3, or Timer T1. It is used as UART #4 Tx on CMv1 for moving monitoring data to the SM.</t>
+  </si>
+  <si>
+    <t>Connection to a GPIO pin on the ZYNQ on the SM. The use is currently undefined, but it can be used for UART #7 Rx or GPIO PC4.  This signal is tied to GND on the original SMv1. It initially has a 270 ohm resistor in series for current limiting.</t>
+  </si>
+  <si>
+    <t>PC5</t>
+  </si>
+  <si>
+    <t>UART for serial data transmitted from the IPMC module on the SM and received by the MCU. Has pads for optional I2C pullup.</t>
+  </si>
+  <si>
+    <t>UART for serial data transmitted from the MCU and received by the IPMC module on the SM. Has pads for optional I2C pullup.</t>
+  </si>
+  <si>
+    <t>UART for serial data transmitted from the ZYNQ module on the SM and received by the MCU. Has pads for optional I2C pullup.</t>
+  </si>
+  <si>
+    <t>UART for serial data transmitted from the MCU and received by the ZYNQ module on the SM. Has pads for optional I2C pullup.</t>
+  </si>
+  <si>
+    <t>I2C module 9 clock,
+UART Module 0 receive,
+GPIO port A bit 0</t>
+  </si>
+  <si>
+    <t>I2C module 7 clock,
+UART Module 3 receive,
+GPIO port A bit 4</t>
+  </si>
+  <si>
+    <t>I2C module 7 data,
+UART Module 3 transmit,
+GPIO port A bit 5</t>
+  </si>
+  <si>
+    <t>I2C module 9 data,
+UART Module 0 transmit,
+GPIO port A bit 1</t>
+  </si>
+  <si>
+    <t>I2C module 8 clock,
+UART Module 4 receive,
+GPIO port A bit 2</t>
+  </si>
+  <si>
+    <t>I2C module 8 data,
+UART Module 4 transmit,
+GPIO port A bit 3</t>
+  </si>
+  <si>
+    <t>Connection to a GPIO pin on the ZYNQ on the SM. The use is currently undefined, but it can be used for UART #7 Tx or GPIO PC5.  This signal is tied to GND on the original SMv1. It initially has a 270 ohm resistor in series for current limiting.</t>
+  </si>
+  <si>
+    <t>UART module 7 transmit,
+GPIO port  C bit 5</t>
+  </si>
+  <si>
+    <t>UART module 7 receive,
+GPIO port  C bit 4</t>
+  </si>
+  <si>
+    <t>I2C module 6 clock,
+UART Module 2 receive,
+GPIO port A bit 6,
+Timer T3</t>
+  </si>
+  <si>
+    <t>I2C module 6 data,
+UART Module 2 transmit,
+GPIO port A bit 7,
+Timer T3</t>
   </si>
 </sst>
 </file>
@@ -2009,8 +2026,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K136"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="I104" sqref="I104"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="K119" sqref="K119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2029,31 +2046,31 @@
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="8"/>
       <c r="B1" s="12" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="9"/>
       <c r="B2" s="12" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="11"/>
       <c r="B3" s="12" t="s">
-        <v>364</v>
+        <v>342</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="10"/>
       <c r="B4" s="12" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="14"/>
       <c r="B5" s="12" t="s">
-        <v>329</v>
+        <v>319</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -2073,13 +2090,13 @@
         <v>4</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>356</v>
+        <v>334</v>
       </c>
       <c r="H8" s="17" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -2087,25 +2104,25 @@
         <v>1</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F9" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="G9" s="13" t="s">
+        <v>213</v>
+      </c>
+      <c r="H9" s="18" t="s">
         <v>212</v>
-      </c>
-      <c r="G9" s="13" t="s">
-        <v>215</v>
-      </c>
-      <c r="H9" s="18" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -2113,25 +2130,25 @@
         <v>2</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F10" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="G10" s="13" t="s">
+        <v>215</v>
+      </c>
+      <c r="H10" s="16" t="s">
         <v>216</v>
-      </c>
-      <c r="G10" s="13" t="s">
-        <v>217</v>
-      </c>
-      <c r="H10" s="16" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -2139,25 +2156,25 @@
         <v>3</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F11" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="G11" s="13" t="s">
         <v>219</v>
       </c>
-      <c r="G11" s="13" t="s">
-        <v>221</v>
-      </c>
       <c r="H11" s="16" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -2165,25 +2182,25 @@
         <v>4</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F12" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="G12" s="4" t="s">
         <v>222</v>
       </c>
-      <c r="G12" s="4" t="s">
-        <v>224</v>
-      </c>
       <c r="H12" s="16" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -2191,25 +2208,25 @@
         <v>5</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="H13" s="16" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -2217,25 +2234,25 @@
         <v>6</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="F14" s="4" t="s">
+        <v>263</v>
+      </c>
+      <c r="G14" s="4" t="s">
         <v>265</v>
       </c>
-      <c r="G14" s="4" t="s">
-        <v>267</v>
-      </c>
       <c r="H14" s="16" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -2243,19 +2260,19 @@
         <v>7</v>
       </c>
       <c r="B15" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E15" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C15" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>57</v>
-      </c>
       <c r="F15" s="4" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>357</v>
+        <v>335</v>
       </c>
       <c r="H15" s="16">
         <v>2.04</v>
@@ -2266,19 +2283,19 @@
         <v>8</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>357</v>
+        <v>335</v>
       </c>
       <c r="H16" s="16">
         <v>3.08</v>
@@ -2289,19 +2306,19 @@
         <v>9</v>
       </c>
       <c r="B17" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E17" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="C17" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>150</v>
-      </c>
       <c r="F17" s="4" t="s">
-        <v>373</v>
+        <v>351</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>374</v>
+        <v>352</v>
       </c>
       <c r="H17" s="16">
         <v>3.08</v>
@@ -2312,19 +2329,19 @@
         <v>10</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C18" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="F18" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="E18" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>58</v>
-      </c>
       <c r="G18" s="4" t="s">
-        <v>358</v>
+        <v>336</v>
       </c>
       <c r="H18" s="16">
         <v>3.08</v>
@@ -2335,25 +2352,25 @@
         <v>11</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="F19" s="4" t="s">
+        <v>266</v>
+      </c>
+      <c r="G19" s="4" t="s">
         <v>268</v>
       </c>
-      <c r="G19" s="4" t="s">
-        <v>270</v>
-      </c>
       <c r="H19" s="16" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -2361,25 +2378,25 @@
         <v>12</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="H20" s="16" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -2387,25 +2404,25 @@
         <v>13</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="H21" s="16" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="K21" s="4"/>
     </row>
@@ -2414,25 +2431,25 @@
         <v>14</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="H22" s="16" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="K22" s="4"/>
     </row>
@@ -2441,25 +2458,25 @@
         <v>15</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="H23" s="16" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="K23" s="4"/>
     </row>
@@ -2468,19 +2485,19 @@
         <v>16</v>
       </c>
       <c r="B24" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E24" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C24" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>57</v>
-      </c>
       <c r="F24" s="4" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>357</v>
+        <v>335</v>
       </c>
       <c r="H24" s="16">
         <v>2.04</v>
@@ -2491,19 +2508,19 @@
         <v>17</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C25" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F25" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="E25" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="F25" s="4" t="s">
-        <v>58</v>
-      </c>
       <c r="G25" s="4" t="s">
-        <v>358</v>
+        <v>336</v>
       </c>
       <c r="H25" s="16">
         <v>2.04</v>
@@ -2514,25 +2531,25 @@
         <v>18</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F26" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="G26" s="13" t="s">
+        <v>233</v>
+      </c>
+      <c r="H26" s="16" t="s">
         <v>234</v>
-      </c>
-      <c r="G26" s="13" t="s">
-        <v>235</v>
-      </c>
-      <c r="H26" s="16" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -2540,25 +2557,25 @@
         <v>19</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="G27" s="13" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="H27" s="16" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -2566,25 +2583,25 @@
         <v>20</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F28" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="G28" s="13" t="s">
         <v>239</v>
       </c>
-      <c r="G28" s="13" t="s">
-        <v>241</v>
-      </c>
       <c r="H28" s="16" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -2592,25 +2609,25 @@
         <v>21</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C29" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F29" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="G29" s="13" t="s">
+        <v>241</v>
+      </c>
+      <c r="H29" s="16" t="s">
         <v>242</v>
-      </c>
-      <c r="G29" s="13" t="s">
-        <v>243</v>
-      </c>
-      <c r="H29" s="16" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -2618,7 +2635,7 @@
         <v>22</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>9</v>
@@ -2627,16 +2644,16 @@
         <v>7</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>375</v>
+        <v>353</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>460</v>
+        <v>436</v>
       </c>
       <c r="H30" s="16" t="s">
-        <v>461</v>
+        <v>437</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="90" x14ac:dyDescent="0.25">
@@ -2644,7 +2661,7 @@
         <v>23</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C31" s="5" t="s">
         <v>6</v>
@@ -2653,65 +2670,65 @@
         <v>7</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>376</v>
+        <v>354</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>443</v>
+        <v>420</v>
       </c>
       <c r="H31" s="16" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="9">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A32" s="15">
         <v>24</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>340</v>
+        <v>468</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>6</v>
+        <v>316</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>7</v>
+        <v>316</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>341</v>
+        <v>480</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>342</v>
+        <v>318</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>321</v>
+        <v>479</v>
       </c>
       <c r="H32" s="16">
         <v>2.0099999999999998</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A33" s="15">
         <v>25</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>326</v>
+        <v>316</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>326</v>
+        <v>316</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>343</v>
+        <v>481</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>344</v>
+        <v>317</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>345</v>
+        <v>467</v>
       </c>
       <c r="H33" s="16">
         <v>2.0099999999999998</v>
@@ -2722,19 +2739,19 @@
         <v>26</v>
       </c>
       <c r="B34" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E34" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C34" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>57</v>
-      </c>
       <c r="F34" s="4" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="G34" s="4" t="s">
-        <v>357</v>
+        <v>335</v>
       </c>
       <c r="H34" s="16">
         <v>2.04</v>
@@ -2745,25 +2762,25 @@
         <v>27</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C35" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="F35" s="4" t="s">
+        <v>269</v>
+      </c>
+      <c r="G35" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="H35" s="16" t="s">
         <v>271</v>
-      </c>
-      <c r="G35" s="4" t="s">
-        <v>272</v>
-      </c>
-      <c r="H35" s="16" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -2771,19 +2788,19 @@
         <v>28</v>
       </c>
       <c r="B36" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E36" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C36" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="E36" s="3" t="s">
-        <v>57</v>
-      </c>
       <c r="F36" s="4" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="G36" s="4" t="s">
-        <v>357</v>
+        <v>335</v>
       </c>
       <c r="H36" s="16">
         <v>2.04</v>
@@ -2794,25 +2811,25 @@
         <v>29</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C37" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="F37" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="G37" s="4" t="s">
         <v>274</v>
       </c>
-      <c r="G37" s="4" t="s">
-        <v>276</v>
-      </c>
       <c r="H37" s="16" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="135" x14ac:dyDescent="0.25">
@@ -2820,7 +2837,7 @@
         <v>30</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C38" s="5" t="s">
         <v>9</v>
@@ -2829,16 +2846,16 @@
         <v>7</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>377</v>
+        <v>355</v>
       </c>
       <c r="G38" s="4" t="s">
-        <v>453</v>
-      </c>
-      <c r="H38" s="16" t="s">
-        <v>452</v>
+        <v>429</v>
+      </c>
+      <c r="H38" s="16">
+        <v>2.0099999999999998</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -2846,7 +2863,7 @@
         <v>31</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C39" s="5" t="s">
         <v>9</v>
@@ -2855,16 +2872,16 @@
         <v>7</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>378</v>
+        <v>356</v>
       </c>
       <c r="G39" s="4" t="s">
-        <v>458</v>
+        <v>434</v>
       </c>
       <c r="H39" s="16" t="s">
-        <v>457</v>
+        <v>433</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -2872,7 +2889,7 @@
         <v>32</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C40" s="5" t="s">
         <v>9</v>
@@ -2881,19 +2898,19 @@
         <v>7</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>379</v>
+        <v>357</v>
       </c>
       <c r="G40" s="4" t="s">
-        <v>459</v>
+        <v>435</v>
       </c>
       <c r="H40" s="16" t="s">
-        <v>457</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A41" s="9">
         <v>33</v>
       </c>
@@ -2907,24 +2924,24 @@
         <v>7</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>16</v>
+        <v>473</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
       <c r="G41" s="4" t="s">
-        <v>320</v>
+        <v>471</v>
       </c>
       <c r="H41" s="16">
         <v>2.0099999999999998</v>
       </c>
     </row>
-    <row r="42" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A42" s="9">
         <v>34</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C42" s="5" t="s">
         <v>6</v>
@@ -2933,76 +2950,76 @@
         <v>7</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>18</v>
+        <v>476</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="G42" s="4" t="s">
-        <v>321</v>
+        <v>472</v>
       </c>
       <c r="H42" s="16">
         <v>2.0099999999999998</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="90" x14ac:dyDescent="0.25">
-      <c r="A43" s="15">
+    <row r="43" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A43" s="9">
         <v>35</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>322</v>
+        <v>314</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>326</v>
+        <v>37</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>326</v>
+        <v>301</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>324</v>
+        <v>477</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>327</v>
+        <v>463</v>
       </c>
       <c r="G43" s="4" t="s">
-        <v>337</v>
+        <v>465</v>
       </c>
       <c r="H43" s="16">
         <v>2.0099999999999998</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="90" x14ac:dyDescent="0.25">
-      <c r="A44" s="15">
+    <row r="44" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A44" s="9">
         <v>36</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>323</v>
+        <v>315</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>326</v>
+        <v>37</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>326</v>
+        <v>301</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>325</v>
+        <v>478</v>
       </c>
       <c r="F44" s="4" t="s">
-        <v>328</v>
+        <v>464</v>
       </c>
       <c r="G44" s="4" t="s">
-        <v>338</v>
+        <v>466</v>
       </c>
       <c r="H44" s="16">
         <v>2.0099999999999998</v>
       </c>
     </row>
-    <row r="45" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A45" s="9">
         <v>37</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C45" s="5" t="s">
         <v>9</v>
@@ -3011,24 +3028,24 @@
         <v>7</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>312</v>
+        <v>474</v>
       </c>
       <c r="F45" s="4" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="G45" s="4" t="s">
-        <v>316</v>
+        <v>469</v>
       </c>
       <c r="H45" s="16">
         <v>2.0099999999999998</v>
       </c>
     </row>
-    <row r="46" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A46" s="9">
         <v>38</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="C46" s="5" t="s">
         <v>6</v>
@@ -3037,13 +3054,13 @@
         <v>7</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>313</v>
+        <v>475</v>
       </c>
       <c r="F46" s="4" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="G46" s="4" t="s">
-        <v>317</v>
+        <v>470</v>
       </c>
       <c r="H46" s="16">
         <v>2.0099999999999998</v>
@@ -3054,19 +3071,19 @@
         <v>39</v>
       </c>
       <c r="B47" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C47" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E47" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C47" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="E47" s="3" t="s">
-        <v>57</v>
-      </c>
       <c r="F47" s="4" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="G47" s="4" t="s">
-        <v>357</v>
+        <v>335</v>
       </c>
       <c r="H47" s="16">
         <v>2.04</v>
@@ -3077,22 +3094,22 @@
         <v>40</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>330</v>
+        <v>320</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>326</v>
+        <v>316</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>326</v>
+        <v>316</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>332</v>
+        <v>482</v>
       </c>
       <c r="F48" s="4" t="s">
-        <v>335</v>
+        <v>323</v>
       </c>
       <c r="G48" s="4" t="s">
-        <v>336</v>
+        <v>324</v>
       </c>
       <c r="H48" s="16">
         <v>2.0099999999999998</v>
@@ -3103,22 +3120,22 @@
         <v>41</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>331</v>
+        <v>321</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>326</v>
+        <v>316</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>326</v>
+        <v>316</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>333</v>
+        <v>483</v>
       </c>
       <c r="F49" s="4" t="s">
-        <v>334</v>
+        <v>322</v>
       </c>
       <c r="G49" s="4" t="s">
-        <v>339</v>
+        <v>325</v>
       </c>
       <c r="H49" s="16">
         <v>2.0099999999999998</v>
@@ -3129,7 +3146,7 @@
         <v>42</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C50" s="5" t="s">
         <v>9</v>
@@ -3138,16 +3155,16 @@
         <v>7</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="F50" s="4" t="s">
-        <v>380</v>
+        <v>358</v>
       </c>
       <c r="G50" s="4" t="s">
-        <v>473</v>
+        <v>449</v>
       </c>
       <c r="H50" s="16" t="s">
-        <v>456</v>
+        <v>432</v>
       </c>
     </row>
     <row r="51" spans="1:8" ht="90" x14ac:dyDescent="0.25">
@@ -3155,7 +3172,7 @@
         <v>43</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C51" s="5" t="s">
         <v>9</v>
@@ -3164,16 +3181,16 @@
         <v>7</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F51" s="4" t="s">
-        <v>381</v>
+        <v>359</v>
       </c>
       <c r="G51" s="4" t="s">
-        <v>474</v>
+        <v>450</v>
       </c>
       <c r="H51" s="16" t="s">
-        <v>456</v>
+        <v>432</v>
       </c>
     </row>
     <row r="52" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -3181,7 +3198,7 @@
         <v>44</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C52" s="5" t="s">
         <v>9</v>
@@ -3190,16 +3207,16 @@
         <v>7</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F52" s="4" t="s">
-        <v>463</v>
+        <v>439</v>
       </c>
       <c r="G52" s="4" t="s">
-        <v>466</v>
+        <v>442</v>
       </c>
       <c r="H52" s="16" t="s">
-        <v>462</v>
+        <v>438</v>
       </c>
     </row>
     <row r="53" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -3207,7 +3224,7 @@
         <v>45</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C53" s="5" t="s">
         <v>9</v>
@@ -3216,16 +3233,16 @@
         <v>7</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="F53" s="4" t="s">
-        <v>382</v>
+        <v>360</v>
       </c>
       <c r="G53" s="4" t="s">
-        <v>465</v>
+        <v>441</v>
       </c>
       <c r="H53" s="16" t="s">
-        <v>462</v>
+        <v>438</v>
       </c>
     </row>
     <row r="54" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -3233,7 +3250,7 @@
         <v>46</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C54" s="5" t="s">
         <v>9</v>
@@ -3242,16 +3259,16 @@
         <v>7</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="F54" s="4" t="s">
-        <v>383</v>
+        <v>361</v>
       </c>
       <c r="G54" s="4" t="s">
-        <v>464</v>
+        <v>440</v>
       </c>
       <c r="H54" s="16" t="s">
-        <v>462</v>
+        <v>438</v>
       </c>
     </row>
     <row r="55" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -3259,19 +3276,19 @@
         <v>47</v>
       </c>
       <c r="B55" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C55" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E55" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C55" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="E55" s="3" t="s">
-        <v>57</v>
-      </c>
       <c r="F55" s="4" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="G55" s="4" t="s">
-        <v>357</v>
+        <v>335</v>
       </c>
       <c r="H55" s="16">
         <v>2.04</v>
@@ -3282,19 +3299,19 @@
         <v>48</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C56" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E56" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F56" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="E56" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="F56" s="4" t="s">
-        <v>58</v>
-      </c>
       <c r="G56" s="4" t="s">
-        <v>358</v>
+        <v>336</v>
       </c>
       <c r="H56" s="16">
         <v>2.04</v>
@@ -3305,25 +3322,25 @@
         <v>49</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="F57" s="4" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="G57" s="4" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="H57" s="16" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="58" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -3331,25 +3348,25 @@
         <v>50</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="F58" s="4" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="G58" s="4" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="H58" s="16" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="59" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -3357,25 +3374,25 @@
         <v>51</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="F59" s="4" t="s">
+        <v>277</v>
+      </c>
+      <c r="G59" s="4" t="s">
         <v>279</v>
       </c>
-      <c r="G59" s="4" t="s">
-        <v>281</v>
-      </c>
       <c r="H59" s="16" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="60" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -3383,25 +3400,25 @@
         <v>52</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="F60" s="4" t="s">
+        <v>278</v>
+      </c>
+      <c r="G60" s="4" t="s">
         <v>280</v>
       </c>
-      <c r="G60" s="4" t="s">
-        <v>282</v>
-      </c>
       <c r="H60" s="16" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="61" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -3409,25 +3426,25 @@
         <v>53</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D61" s="5" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="F61" s="4" t="s">
+        <v>281</v>
+      </c>
+      <c r="G61" s="4" t="s">
         <v>283</v>
       </c>
-      <c r="G61" s="4" t="s">
-        <v>285</v>
-      </c>
       <c r="H61" s="16" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="62" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -3435,25 +3452,25 @@
         <v>54</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C62" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D62" s="5" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="E62" s="3" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="F62" s="4" t="s">
+        <v>282</v>
+      </c>
+      <c r="G62" s="4" t="s">
         <v>284</v>
       </c>
-      <c r="G62" s="4" t="s">
-        <v>286</v>
-      </c>
       <c r="H62" s="16" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="63" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -3461,25 +3478,25 @@
         <v>55</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C63" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D63" s="5" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="E63" s="3" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="F63" s="4" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="G63" s="4" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="H63" s="16" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="64" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -3487,25 +3504,25 @@
         <v>56</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D64" s="5" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="E64" s="3" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="F64" s="4" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="G64" s="4" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="H64" s="16" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="65" spans="1:11" ht="90" x14ac:dyDescent="0.25">
@@ -3513,7 +3530,7 @@
         <v>57</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C65" s="5" t="s">
         <v>9</v>
@@ -3522,16 +3539,16 @@
         <v>7</v>
       </c>
       <c r="E65" s="3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="F65" s="4" t="s">
-        <v>384</v>
+        <v>362</v>
       </c>
       <c r="G65" s="4" t="s">
-        <v>471</v>
+        <v>447</v>
       </c>
       <c r="H65" s="16" t="s">
-        <v>455</v>
+        <v>431</v>
       </c>
     </row>
     <row r="66" spans="1:11" ht="90" x14ac:dyDescent="0.25">
@@ -3539,7 +3556,7 @@
         <v>58</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C66" s="5" t="s">
         <v>9</v>
@@ -3548,16 +3565,16 @@
         <v>7</v>
       </c>
       <c r="E66" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="F66" s="4" t="s">
-        <v>385</v>
+        <v>363</v>
       </c>
       <c r="G66" s="4" t="s">
-        <v>472</v>
+        <v>448</v>
       </c>
       <c r="H66" s="16" t="s">
-        <v>455</v>
+        <v>431</v>
       </c>
     </row>
     <row r="67" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -3565,7 +3582,7 @@
         <v>59</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C67" s="5" t="s">
         <v>9</v>
@@ -3574,16 +3591,16 @@
         <v>7</v>
       </c>
       <c r="E67" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="F67" s="4" t="s">
-        <v>386</v>
+        <v>364</v>
       </c>
       <c r="G67" s="4" t="s">
-        <v>467</v>
+        <v>443</v>
       </c>
       <c r="H67" s="16" t="s">
-        <v>470</v>
+        <v>446</v>
       </c>
     </row>
     <row r="68" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -3591,7 +3608,7 @@
         <v>60</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C68" s="5" t="s">
         <v>9</v>
@@ -3600,16 +3617,16 @@
         <v>7</v>
       </c>
       <c r="E68" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="F68" s="4" t="s">
-        <v>387</v>
+        <v>365</v>
       </c>
       <c r="G68" s="4" t="s">
-        <v>468</v>
+        <v>444</v>
       </c>
       <c r="H68" s="16" t="s">
-        <v>470</v>
+        <v>446</v>
       </c>
     </row>
     <row r="69" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -3617,7 +3634,7 @@
         <v>61</v>
       </c>
       <c r="B69" s="5" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C69" s="5" t="s">
         <v>9</v>
@@ -3626,16 +3643,16 @@
         <v>7</v>
       </c>
       <c r="E69" s="3" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="F69" s="4" t="s">
-        <v>388</v>
+        <v>366</v>
       </c>
       <c r="G69" s="4" t="s">
-        <v>469</v>
+        <v>445</v>
       </c>
       <c r="H69" s="16" t="s">
-        <v>470</v>
+        <v>446</v>
       </c>
     </row>
     <row r="70" spans="1:11" ht="90" x14ac:dyDescent="0.25">
@@ -3643,7 +3660,7 @@
         <v>62</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C70" s="5" t="s">
         <v>9</v>
@@ -3652,16 +3669,16 @@
         <v>7</v>
       </c>
       <c r="E70" s="3" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="F70" s="4" t="s">
-        <v>428</v>
+        <v>406</v>
       </c>
       <c r="G70" s="4" t="s">
-        <v>437</v>
+        <v>414</v>
       </c>
       <c r="H70" s="16" t="s">
-        <v>427</v>
+        <v>405</v>
       </c>
       <c r="K70" s="4"/>
     </row>
@@ -3670,19 +3687,19 @@
         <v>63</v>
       </c>
       <c r="B71" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C71" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E71" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C71" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="E71" s="3" t="s">
-        <v>57</v>
-      </c>
       <c r="F71" s="4" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="G71" s="4" t="s">
-        <v>357</v>
+        <v>335</v>
       </c>
       <c r="H71" s="16">
         <v>2.04</v>
@@ -3694,7 +3711,7 @@
         <v>64</v>
       </c>
       <c r="B72" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C72" s="5" t="s">
         <v>9</v>
@@ -3703,13 +3720,13 @@
         <v>7</v>
       </c>
       <c r="E72" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F72" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G72" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H72" s="16">
         <v>2.04</v>
@@ -3720,7 +3737,7 @@
         <v>65</v>
       </c>
       <c r="B73" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C73" s="5" t="s">
         <v>6</v>
@@ -3729,13 +3746,13 @@
         <v>7</v>
       </c>
       <c r="E73" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F73" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G73" s="4" t="s">
-        <v>366</v>
+        <v>344</v>
       </c>
       <c r="H73" s="16">
         <v>2.04</v>
@@ -3746,22 +3763,22 @@
         <v>66</v>
       </c>
       <c r="B74" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C74" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D74" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E74" s="3" t="s">
+        <v>349</v>
+      </c>
+      <c r="F74" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E74" s="3" t="s">
-        <v>371</v>
-      </c>
-      <c r="F74" s="4" t="s">
-        <v>26</v>
-      </c>
       <c r="G74" s="4" t="s">
-        <v>370</v>
+        <v>348</v>
       </c>
       <c r="H74" s="16">
         <v>2.04</v>
@@ -3772,22 +3789,22 @@
         <v>67</v>
       </c>
       <c r="B75" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C75" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D75" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>372</v>
+        <v>350</v>
       </c>
       <c r="F75" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G75" s="4" t="s">
-        <v>370</v>
+        <v>348</v>
       </c>
       <c r="H75" s="16">
         <v>2.04</v>
@@ -3798,19 +3815,19 @@
         <v>68</v>
       </c>
       <c r="B76" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C76" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E76" s="3" t="s">
-        <v>359</v>
+        <v>337</v>
       </c>
       <c r="F76" s="4" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="G76" s="4" t="s">
-        <v>360</v>
+        <v>338</v>
       </c>
       <c r="H76" s="16">
         <v>2.04</v>
@@ -3821,19 +3838,19 @@
         <v>69</v>
       </c>
       <c r="B77" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C77" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E77" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C77" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="E77" s="3" t="s">
-        <v>57</v>
-      </c>
       <c r="F77" s="4" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="G77" s="4" t="s">
-        <v>357</v>
+        <v>335</v>
       </c>
       <c r="H77" s="16">
         <v>2.04</v>
@@ -3844,7 +3861,7 @@
         <v>70</v>
       </c>
       <c r="B78" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C78" s="5" t="s">
         <v>9</v>
@@ -3853,13 +3870,13 @@
         <v>7</v>
       </c>
       <c r="E78" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F78" s="4" t="s">
-        <v>365</v>
+        <v>343</v>
       </c>
       <c r="G78" s="4" t="s">
-        <v>438</v>
+        <v>415</v>
       </c>
       <c r="H78" s="16">
         <v>2.04</v>
@@ -3870,7 +3887,7 @@
         <v>71</v>
       </c>
       <c r="B79" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C79" s="5" t="s">
         <v>9</v>
@@ -3879,16 +3896,16 @@
         <v>7</v>
       </c>
       <c r="E79" s="3" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F79" s="4" t="s">
-        <v>429</v>
+        <v>407</v>
       </c>
       <c r="G79" s="4" t="s">
-        <v>444</v>
+        <v>421</v>
       </c>
       <c r="H79" s="16" t="s">
-        <v>430</v>
+        <v>408</v>
       </c>
     </row>
     <row r="80" spans="1:11" ht="90" x14ac:dyDescent="0.25">
@@ -3896,7 +3913,7 @@
         <v>72</v>
       </c>
       <c r="B80" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C80" s="5" t="s">
         <v>9</v>
@@ -3905,16 +3922,16 @@
         <v>7</v>
       </c>
       <c r="E80" s="3" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="F80" s="4" t="s">
-        <v>405</v>
+        <v>383</v>
       </c>
       <c r="G80" s="4" t="s">
-        <v>413</v>
+        <v>391</v>
       </c>
       <c r="H80" s="16" t="s">
-        <v>406</v>
+        <v>384</v>
       </c>
     </row>
     <row r="81" spans="1:11" ht="90" x14ac:dyDescent="0.25">
@@ -3922,7 +3939,7 @@
         <v>73</v>
       </c>
       <c r="B81" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C81" s="5" t="s">
         <v>9</v>
@@ -3931,16 +3948,16 @@
         <v>7</v>
       </c>
       <c r="E81" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="F81" s="4" t="s">
-        <v>407</v>
+        <v>385</v>
       </c>
       <c r="G81" s="4" t="s">
-        <v>414</v>
+        <v>392</v>
       </c>
       <c r="H81" s="16" t="s">
-        <v>408</v>
+        <v>386</v>
       </c>
     </row>
     <row r="82" spans="1:11" ht="90" x14ac:dyDescent="0.25">
@@ -3948,7 +3965,7 @@
         <v>74</v>
       </c>
       <c r="B82" s="5" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C82" s="5" t="s">
         <v>6</v>
@@ -3957,16 +3974,16 @@
         <v>7</v>
       </c>
       <c r="E82" s="3" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="F82" s="4" t="s">
-        <v>409</v>
+        <v>387</v>
       </c>
       <c r="G82" s="4" t="s">
-        <v>415</v>
+        <v>393</v>
       </c>
       <c r="H82" s="16" t="s">
-        <v>406</v>
+        <v>384</v>
       </c>
     </row>
     <row r="83" spans="1:11" ht="90" x14ac:dyDescent="0.25">
@@ -3974,7 +3991,7 @@
         <v>75</v>
       </c>
       <c r="B83" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C83" s="5" t="s">
         <v>6</v>
@@ -3983,16 +4000,16 @@
         <v>7</v>
       </c>
       <c r="E83" s="3" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="F83" s="4" t="s">
-        <v>410</v>
+        <v>388</v>
       </c>
       <c r="G83" s="4" t="s">
-        <v>416</v>
+        <v>394</v>
       </c>
       <c r="H83" s="16" t="s">
-        <v>406</v>
+        <v>384</v>
       </c>
     </row>
     <row r="84" spans="1:11" ht="90" x14ac:dyDescent="0.25">
@@ -4000,7 +4017,7 @@
         <v>76</v>
       </c>
       <c r="B84" s="5" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C84" s="5" t="s">
         <v>6</v>
@@ -4009,16 +4026,16 @@
         <v>7</v>
       </c>
       <c r="E84" s="3" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="F84" s="4" t="s">
-        <v>389</v>
+        <v>367</v>
       </c>
       <c r="G84" s="4" t="s">
-        <v>454</v>
-      </c>
-      <c r="H84" s="16" t="s">
-        <v>452</v>
+        <v>430</v>
+      </c>
+      <c r="H84" s="16">
+        <v>2.0099999999999998</v>
       </c>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.25">
@@ -4026,7 +4043,7 @@
         <v>77</v>
       </c>
       <c r="B85" s="5" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C85" s="5" t="s">
         <v>6</v>
@@ -4035,10 +4052,10 @@
         <v>7</v>
       </c>
       <c r="E85" s="3" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="F85" s="4" t="s">
-        <v>390</v>
+        <v>368</v>
       </c>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.25">
@@ -4046,7 +4063,7 @@
         <v>78</v>
       </c>
       <c r="B86" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C86" s="5" t="s">
         <v>6</v>
@@ -4055,10 +4072,10 @@
         <v>7</v>
       </c>
       <c r="E86" s="3" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="F86" s="4" t="s">
-        <v>391</v>
+        <v>369</v>
       </c>
       <c r="K86" s="4"/>
     </row>
@@ -4067,19 +4084,19 @@
         <v>79</v>
       </c>
       <c r="B87" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C87" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E87" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C87" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="E87" s="3" t="s">
-        <v>57</v>
-      </c>
       <c r="F87" s="4" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="G87" s="4" t="s">
-        <v>357</v>
+        <v>335</v>
       </c>
       <c r="H87" s="16">
         <v>2.04</v>
@@ -4090,19 +4107,19 @@
         <v>80</v>
       </c>
       <c r="B88" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C88" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E88" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F88" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="E88" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="F88" s="4" t="s">
-        <v>58</v>
-      </c>
       <c r="G88" s="4" t="s">
-        <v>358</v>
+        <v>336</v>
       </c>
       <c r="H88" s="16">
         <v>2.04</v>
@@ -4113,7 +4130,7 @@
         <v>81</v>
       </c>
       <c r="B89" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C89" s="5" t="s">
         <v>6</v>
@@ -4122,16 +4139,16 @@
         <v>7</v>
       </c>
       <c r="E89" s="3" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F89" s="4" t="s">
-        <v>392</v>
+        <v>370</v>
       </c>
       <c r="G89" s="4" t="s">
-        <v>475</v>
+        <v>451</v>
       </c>
       <c r="H89" s="16" t="s">
-        <v>456</v>
+        <v>432</v>
       </c>
       <c r="K89" s="4"/>
     </row>
@@ -4140,7 +4157,7 @@
         <v>82</v>
       </c>
       <c r="B90" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C90" s="5" t="s">
         <v>6</v>
@@ -4149,16 +4166,16 @@
         <v>7</v>
       </c>
       <c r="E90" s="3" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F90" s="4" t="s">
-        <v>393</v>
+        <v>371</v>
       </c>
       <c r="G90" s="4" t="s">
-        <v>480</v>
+        <v>456</v>
       </c>
       <c r="H90" s="16" t="s">
-        <v>477</v>
+        <v>453</v>
       </c>
       <c r="K90" s="4"/>
     </row>
@@ -4167,7 +4184,7 @@
         <v>83</v>
       </c>
       <c r="B91" s="5" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C91" s="5" t="s">
         <v>6</v>
@@ -4176,16 +4193,16 @@
         <v>7</v>
       </c>
       <c r="E91" s="3" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="F91" s="4" t="s">
-        <v>394</v>
+        <v>372</v>
       </c>
       <c r="G91" s="4" t="s">
-        <v>479</v>
+        <v>455</v>
       </c>
       <c r="H91" s="16" t="s">
-        <v>477</v>
+        <v>453</v>
       </c>
     </row>
     <row r="92" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -4193,7 +4210,7 @@
         <v>84</v>
       </c>
       <c r="B92" s="5" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C92" s="5" t="s">
         <v>6</v>
@@ -4202,16 +4219,16 @@
         <v>7</v>
       </c>
       <c r="E92" s="3" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="F92" s="4" t="s">
-        <v>395</v>
+        <v>373</v>
       </c>
       <c r="G92" s="4" t="s">
-        <v>478</v>
+        <v>454</v>
       </c>
       <c r="H92" s="16" t="s">
-        <v>477</v>
+        <v>453</v>
       </c>
     </row>
     <row r="93" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -4219,7 +4236,7 @@
         <v>85</v>
       </c>
       <c r="B93" s="5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C93" s="5" t="s">
         <v>6</v>
@@ -4228,16 +4245,16 @@
         <v>7</v>
       </c>
       <c r="E93" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="F93" s="4" t="s">
-        <v>396</v>
+        <v>374</v>
       </c>
       <c r="G93" s="4" t="s">
-        <v>476</v>
+        <v>452</v>
       </c>
       <c r="H93" s="16" t="s">
-        <v>455</v>
+        <v>431</v>
       </c>
     </row>
     <row r="94" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -4245,7 +4262,7 @@
         <v>86</v>
       </c>
       <c r="B94" s="5" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C94" s="5" t="s">
         <v>6</v>
@@ -4254,16 +4271,16 @@
         <v>7</v>
       </c>
       <c r="E94" s="3" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="F94" s="4" t="s">
-        <v>397</v>
+        <v>375</v>
       </c>
       <c r="G94" s="4" t="s">
-        <v>481</v>
+        <v>457</v>
       </c>
       <c r="H94" s="16" t="s">
-        <v>482</v>
+        <v>458</v>
       </c>
     </row>
     <row r="95" spans="1:11" ht="75" x14ac:dyDescent="0.25">
@@ -4271,19 +4288,19 @@
         <v>87</v>
       </c>
       <c r="B95" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C95" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E95" s="3" t="s">
-        <v>362</v>
+        <v>340</v>
       </c>
       <c r="F95" s="4" t="s">
-        <v>361</v>
+        <v>339</v>
       </c>
       <c r="G95" s="3" t="s">
-        <v>363</v>
+        <v>341</v>
       </c>
       <c r="H95" s="16">
         <v>2.04</v>
@@ -4294,22 +4311,22 @@
         <v>88</v>
       </c>
       <c r="B96" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C96" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D96" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E96" s="3" t="s">
-        <v>368</v>
+        <v>346</v>
       </c>
       <c r="F96" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G96" s="4" t="s">
-        <v>367</v>
+        <v>345</v>
       </c>
       <c r="H96" s="16">
         <v>2.04</v>
@@ -4320,22 +4337,22 @@
         <v>89</v>
       </c>
       <c r="B97" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C97" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D97" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E97" s="3" t="s">
-        <v>369</v>
+        <v>347</v>
       </c>
       <c r="F97" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G97" s="4" t="s">
-        <v>367</v>
+        <v>345</v>
       </c>
       <c r="H97" s="16">
         <v>2.04</v>
@@ -4346,19 +4363,19 @@
         <v>90</v>
       </c>
       <c r="B98" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C98" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E98" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C98" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="E98" s="3" t="s">
-        <v>57</v>
-      </c>
       <c r="F98" s="4" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="G98" s="4" t="s">
-        <v>357</v>
+        <v>335</v>
       </c>
       <c r="H98" s="16">
         <v>2.04</v>
@@ -4369,22 +4386,22 @@
         <v>91</v>
       </c>
       <c r="B99" s="5" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C99" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D99" s="5" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="E99" s="3" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="F99" s="4" t="s">
-        <v>347</v>
+        <v>462</v>
       </c>
       <c r="G99" s="4" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="H99" s="16">
         <v>2.0099999999999998</v>
@@ -4395,22 +4412,22 @@
         <v>92</v>
       </c>
       <c r="B100" s="5" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C100" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D100" s="5" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="E100" s="3" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="F100" s="4" t="s">
-        <v>346</v>
+        <v>461</v>
       </c>
       <c r="G100" s="4" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="H100" s="16">
         <v>2.0099999999999998</v>
@@ -4421,7 +4438,7 @@
         <v>93</v>
       </c>
       <c r="B101" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C101" s="5" t="s">
         <v>6</v>
@@ -4430,16 +4447,16 @@
         <v>7</v>
       </c>
       <c r="E101" s="3" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="F101" s="4" t="s">
-        <v>398</v>
+        <v>376</v>
       </c>
       <c r="G101" s="4" t="s">
-        <v>483</v>
+        <v>459</v>
       </c>
       <c r="H101" s="16" t="s">
-        <v>482</v>
+        <v>458</v>
       </c>
     </row>
     <row r="102" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -4447,7 +4464,7 @@
         <v>94</v>
       </c>
       <c r="B102" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C102" s="5" t="s">
         <v>6</v>
@@ -4456,16 +4473,16 @@
         <v>7</v>
       </c>
       <c r="E102" s="3" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="F102" s="4" t="s">
-        <v>399</v>
+        <v>377</v>
       </c>
       <c r="G102" s="4" t="s">
-        <v>484</v>
+        <v>460</v>
       </c>
       <c r="H102" s="16" t="s">
-        <v>482</v>
+        <v>458</v>
       </c>
     </row>
     <row r="103" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -4473,25 +4490,25 @@
         <v>95</v>
       </c>
       <c r="B103" s="5" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C103" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D103" s="5" t="s">
+        <v>301</v>
+      </c>
+      <c r="E103" s="3" t="s">
         <v>303</v>
       </c>
-      <c r="E103" s="3" t="s">
-        <v>305</v>
-      </c>
       <c r="F103" s="4" t="s">
+        <v>292</v>
+      </c>
+      <c r="G103" s="4" t="s">
         <v>294</v>
       </c>
-      <c r="G103" s="4" t="s">
-        <v>296</v>
-      </c>
       <c r="H103" s="16" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="104" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -4499,25 +4516,25 @@
         <v>96</v>
       </c>
       <c r="B104" s="5" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="C104" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D104" s="5" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="E104" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="F104" s="4" t="s">
         <v>293</v>
       </c>
-      <c r="F104" s="4" t="s">
+      <c r="G104" s="4" t="s">
         <v>295</v>
       </c>
-      <c r="G104" s="4" t="s">
-        <v>297</v>
-      </c>
       <c r="H104" s="16" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="105" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -4537,10 +4554,10 @@
         <v>11</v>
       </c>
       <c r="F105" s="3" t="s">
-        <v>348</v>
+        <v>326</v>
       </c>
       <c r="G105" s="4" t="s">
-        <v>352</v>
+        <v>330</v>
       </c>
       <c r="H105" s="16">
         <v>2.0299999999999998</v>
@@ -4560,13 +4577,13 @@
         <v>7</v>
       </c>
       <c r="E106" s="3" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="F106" s="3" t="s">
-        <v>349</v>
+        <v>327</v>
       </c>
       <c r="G106" s="4" t="s">
-        <v>353</v>
+        <v>331</v>
       </c>
       <c r="H106" s="16">
         <v>2.0299999999999998</v>
@@ -4589,10 +4606,10 @@
         <v>10</v>
       </c>
       <c r="F107" s="3" t="s">
-        <v>350</v>
+        <v>328</v>
       </c>
       <c r="G107" s="4" t="s">
-        <v>354</v>
+        <v>332</v>
       </c>
       <c r="H107" s="16">
         <v>2.0299999999999998</v>
@@ -4615,10 +4632,10 @@
         <v>14</v>
       </c>
       <c r="F108" s="3" t="s">
-        <v>351</v>
+        <v>329</v>
       </c>
       <c r="G108" s="4" t="s">
-        <v>355</v>
+        <v>333</v>
       </c>
       <c r="H108" s="16">
         <v>2.0299999999999998</v>
@@ -4629,19 +4646,19 @@
         <v>101</v>
       </c>
       <c r="B109" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C109" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E109" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C109" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="E109" s="3" t="s">
-        <v>57</v>
-      </c>
       <c r="F109" s="4" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="G109" s="4" t="s">
-        <v>357</v>
+        <v>335</v>
       </c>
       <c r="H109" s="16">
         <v>2.04</v>
@@ -4652,7 +4669,7 @@
         <v>102</v>
       </c>
       <c r="B110" s="5" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C110" s="5" t="s">
         <v>6</v>
@@ -4661,16 +4678,16 @@
         <v>7</v>
       </c>
       <c r="E110" s="3" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="F110" s="4" t="s">
-        <v>400</v>
+        <v>378</v>
       </c>
       <c r="G110" s="4" t="s">
-        <v>445</v>
+        <v>422</v>
       </c>
       <c r="H110" s="16" t="s">
-        <v>431</v>
+        <v>409</v>
       </c>
     </row>
     <row r="111" spans="1:8" ht="90" x14ac:dyDescent="0.25">
@@ -4678,7 +4695,7 @@
         <v>103</v>
       </c>
       <c r="B111" s="5" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C111" s="5" t="s">
         <v>6</v>
@@ -4687,16 +4704,16 @@
         <v>7</v>
       </c>
       <c r="E111" s="3" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F111" s="4" t="s">
-        <v>401</v>
+        <v>379</v>
       </c>
       <c r="G111" s="4" t="s">
-        <v>440</v>
+        <v>417</v>
       </c>
       <c r="H111" s="16" t="s">
-        <v>427</v>
+        <v>405</v>
       </c>
     </row>
     <row r="112" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -4704,7 +4721,7 @@
         <v>104</v>
       </c>
       <c r="B112" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C112" s="5" t="s">
         <v>6</v>
@@ -4713,16 +4730,16 @@
         <v>7</v>
       </c>
       <c r="E112" s="3" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="F112" s="4" t="s">
-        <v>417</v>
+        <v>395</v>
       </c>
       <c r="G112" s="4" t="s">
-        <v>446</v>
+        <v>423</v>
       </c>
       <c r="H112" s="16" t="s">
-        <v>420</v>
+        <v>398</v>
       </c>
     </row>
     <row r="113" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -4730,7 +4747,7 @@
         <v>105</v>
       </c>
       <c r="B113" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C113" s="5" t="s">
         <v>6</v>
@@ -4739,16 +4756,16 @@
         <v>7</v>
       </c>
       <c r="E113" s="3" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="F113" s="4" t="s">
-        <v>418</v>
+        <v>396</v>
       </c>
       <c r="G113" s="4" t="s">
-        <v>447</v>
+        <v>424</v>
       </c>
       <c r="H113" s="16" t="s">
-        <v>420</v>
+        <v>398</v>
       </c>
     </row>
     <row r="114" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -4756,7 +4773,7 @@
         <v>106</v>
       </c>
       <c r="B114" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C114" s="5" t="s">
         <v>6</v>
@@ -4765,16 +4782,16 @@
         <v>7</v>
       </c>
       <c r="E114" s="3" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="F114" s="4" t="s">
-        <v>419</v>
+        <v>397</v>
       </c>
       <c r="G114" s="4" t="s">
-        <v>448</v>
+        <v>425</v>
       </c>
       <c r="H114" s="16" t="s">
-        <v>420</v>
+        <v>398</v>
       </c>
       <c r="K114" s="4"/>
     </row>
@@ -4783,7 +4800,7 @@
         <v>107</v>
       </c>
       <c r="B115" s="5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C115" s="5" t="s">
         <v>6</v>
@@ -4792,16 +4809,16 @@
         <v>7</v>
       </c>
       <c r="E115" s="3" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F115" s="4" t="s">
-        <v>450</v>
+        <v>427</v>
       </c>
       <c r="G115" s="4" t="s">
-        <v>451</v>
+        <v>428</v>
       </c>
       <c r="H115" s="16" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="116" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -4809,7 +4826,7 @@
         <v>108</v>
       </c>
       <c r="B116" s="5" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C116" s="5" t="s">
         <v>6</v>
@@ -4818,16 +4835,16 @@
         <v>7</v>
       </c>
       <c r="E116" s="3" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F116" s="4" t="s">
-        <v>402</v>
+        <v>380</v>
       </c>
       <c r="G116" s="4" t="s">
-        <v>449</v>
-      </c>
-      <c r="H116" s="16" t="s">
-        <v>432</v>
+        <v>426</v>
+      </c>
+      <c r="H116" s="16">
+        <v>2.0299999999999998</v>
       </c>
     </row>
     <row r="117" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -4835,7 +4852,7 @@
         <v>109</v>
       </c>
       <c r="B117" s="5" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C117" s="5" t="s">
         <v>6</v>
@@ -4844,16 +4861,16 @@
         <v>7</v>
       </c>
       <c r="E117" s="3" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F117" s="4" t="s">
-        <v>433</v>
+        <v>410</v>
       </c>
       <c r="G117" s="4" t="s">
-        <v>441</v>
-      </c>
-      <c r="H117" s="16" t="s">
-        <v>432</v>
+        <v>418</v>
+      </c>
+      <c r="H117" s="16">
+        <v>2.0299999999999998</v>
       </c>
     </row>
     <row r="118" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -4861,7 +4878,7 @@
         <v>110</v>
       </c>
       <c r="B118" s="5" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C118" s="5" t="s">
         <v>6</v>
@@ -4870,16 +4887,16 @@
         <v>7</v>
       </c>
       <c r="E118" s="3" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F118" s="4" t="s">
-        <v>434</v>
+        <v>411</v>
       </c>
       <c r="G118" s="4" t="s">
-        <v>442</v>
-      </c>
-      <c r="H118" s="16" t="s">
-        <v>432</v>
+        <v>419</v>
+      </c>
+      <c r="H118" s="16">
+        <v>2.0299999999999998</v>
       </c>
     </row>
     <row r="119" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -4887,25 +4904,25 @@
         <v>111</v>
       </c>
       <c r="B119" s="5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C119" s="5" t="s">
-        <v>326</v>
+        <v>316</v>
       </c>
       <c r="D119" s="5" t="s">
-        <v>326</v>
+        <v>316</v>
       </c>
       <c r="E119" s="3" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="F119" s="4" t="s">
-        <v>403</v>
+        <v>381</v>
       </c>
       <c r="G119" s="4" t="s">
-        <v>439</v>
+        <v>416</v>
       </c>
       <c r="H119" s="16" t="s">
-        <v>420</v>
+        <v>398</v>
       </c>
       <c r="K119" s="4"/>
     </row>
@@ -4914,25 +4931,25 @@
         <v>112</v>
       </c>
       <c r="B120" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C120" s="5" t="s">
-        <v>326</v>
+        <v>316</v>
       </c>
       <c r="D120" s="5" t="s">
-        <v>326</v>
+        <v>316</v>
       </c>
       <c r="E120" s="3" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="F120" s="4" t="s">
-        <v>404</v>
+        <v>382</v>
       </c>
       <c r="G120" s="4" t="s">
-        <v>439</v>
+        <v>416</v>
       </c>
       <c r="H120" s="16" t="s">
-        <v>420</v>
+        <v>398</v>
       </c>
       <c r="K120" s="4"/>
     </row>
@@ -4941,19 +4958,19 @@
         <v>113</v>
       </c>
       <c r="B121" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C121" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E121" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C121" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="E121" s="3" t="s">
-        <v>57</v>
-      </c>
       <c r="F121" s="4" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="G121" s="4" t="s">
-        <v>357</v>
+        <v>335</v>
       </c>
       <c r="H121" s="16">
         <v>2.04</v>
@@ -4964,19 +4981,19 @@
         <v>114</v>
       </c>
       <c r="B122" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C122" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E122" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F122" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="E122" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="F122" s="4" t="s">
-        <v>58</v>
-      </c>
       <c r="G122" s="4" t="s">
-        <v>358</v>
+        <v>336</v>
       </c>
       <c r="H122" s="16">
         <v>2.04</v>
@@ -4987,19 +5004,19 @@
         <v>115</v>
       </c>
       <c r="B123" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C123" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E123" s="3" t="s">
-        <v>362</v>
+        <v>340</v>
       </c>
       <c r="F123" s="4" t="s">
-        <v>361</v>
+        <v>339</v>
       </c>
       <c r="G123" s="3" t="s">
-        <v>363</v>
+        <v>341</v>
       </c>
       <c r="H123" s="16">
         <v>2.04</v>
@@ -5010,7 +5027,7 @@
         <v>116</v>
       </c>
       <c r="B124" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C124" s="5" t="s">
         <v>9</v>
@@ -5019,16 +5036,16 @@
         <v>7</v>
       </c>
       <c r="E124" s="3" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="F124" s="4" t="s">
-        <v>411</v>
+        <v>389</v>
       </c>
       <c r="G124" s="4" t="s">
-        <v>435</v>
+        <v>412</v>
       </c>
       <c r="H124" s="16" t="s">
-        <v>406</v>
+        <v>384</v>
       </c>
     </row>
     <row r="125" spans="1:11" ht="120" x14ac:dyDescent="0.25">
@@ -5036,7 +5053,7 @@
         <v>117</v>
       </c>
       <c r="B125" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C125" s="5" t="s">
         <v>9</v>
@@ -5045,16 +5062,16 @@
         <v>7</v>
       </c>
       <c r="E125" s="3" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="F125" s="4" t="s">
-        <v>412</v>
+        <v>390</v>
       </c>
       <c r="G125" s="4" t="s">
-        <v>436</v>
+        <v>413</v>
       </c>
       <c r="H125" s="16" t="s">
-        <v>408</v>
+        <v>386</v>
       </c>
     </row>
     <row r="126" spans="1:11" ht="75" x14ac:dyDescent="0.25">
@@ -5062,7 +5079,7 @@
         <v>118</v>
       </c>
       <c r="B126" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C126" s="5" t="s">
         <v>9</v>
@@ -5071,16 +5088,16 @@
         <v>7</v>
       </c>
       <c r="E126" s="3" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="F126" s="4" t="s">
-        <v>421</v>
+        <v>399</v>
       </c>
       <c r="G126" s="4" t="s">
-        <v>424</v>
+        <v>402</v>
       </c>
       <c r="H126" s="16" t="s">
-        <v>423</v>
+        <v>401</v>
       </c>
     </row>
     <row r="127" spans="1:11" ht="75" x14ac:dyDescent="0.25">
@@ -5088,7 +5105,7 @@
         <v>119</v>
       </c>
       <c r="B127" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C127" s="5" t="s">
         <v>9</v>
@@ -5097,16 +5114,16 @@
         <v>7</v>
       </c>
       <c r="E127" s="3" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="F127" s="4" t="s">
-        <v>422</v>
+        <v>400</v>
       </c>
       <c r="G127" s="4" t="s">
-        <v>426</v>
+        <v>404</v>
       </c>
       <c r="H127" s="16" t="s">
-        <v>425</v>
+        <v>403</v>
       </c>
     </row>
     <row r="128" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -5114,25 +5131,25 @@
         <v>120</v>
       </c>
       <c r="B128" s="5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C128" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D128" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E128" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F128" s="4" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="G128" s="4" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="H128" s="16" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="129" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -5140,25 +5157,25 @@
         <v>121</v>
       </c>
       <c r="B129" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C129" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D129" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E129" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F129" s="4" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="G129" s="4" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="H129" s="16" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="130" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -5166,19 +5183,19 @@
         <v>122</v>
       </c>
       <c r="B130" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C130" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E130" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C130" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="E130" s="3" t="s">
-        <v>57</v>
-      </c>
       <c r="F130" s="4" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="G130" s="4" t="s">
-        <v>357</v>
+        <v>335</v>
       </c>
       <c r="H130" s="16">
         <v>2.04</v>
@@ -5189,25 +5206,25 @@
         <v>123</v>
       </c>
       <c r="B131" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C131" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D131" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E131" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F131" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="G131" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="H131" s="16" t="s">
         <v>256</v>
-      </c>
-      <c r="G131" s="4" t="s">
-        <v>257</v>
-      </c>
-      <c r="H131" s="16" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="132" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -5215,25 +5232,25 @@
         <v>124</v>
       </c>
       <c r="B132" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C132" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D132" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E132" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F132" s="4" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="G132" s="4" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="H132" s="16" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="133" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -5241,25 +5258,25 @@
         <v>125</v>
       </c>
       <c r="B133" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C133" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D133" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E133" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F133" s="4" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="G133" s="4" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="H133" s="16" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="134" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -5267,25 +5284,25 @@
         <v>126</v>
       </c>
       <c r="B134" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C134" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D134" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E134" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F134" s="4" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="G134" s="4" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="H134" s="16" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="135" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -5293,25 +5310,25 @@
         <v>127</v>
       </c>
       <c r="B135" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C135" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D135" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E135" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F135" s="4" t="s">
+        <v>249</v>
+      </c>
+      <c r="G135" s="4" t="s">
+        <v>250</v>
+      </c>
+      <c r="H135" s="16" t="s">
         <v>251</v>
-      </c>
-      <c r="G135" s="4" t="s">
-        <v>252</v>
-      </c>
-      <c r="H135" s="16" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="136" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -5319,25 +5336,25 @@
         <v>128</v>
       </c>
       <c r="B136" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C136" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D136" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E136" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F136" s="4" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="G136" s="4" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="H136" s="16" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated schematic page numbers
</commit_message>
<xml_diff>
--- a/Docs/CMv2_TM4C_controller_pin_specs.xlsx
+++ b/Docs/CMv2_TM4C_controller_pin_specs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\6089-119_CM_2xVU13P\GitHub\Cornell_CM_Rev2_HW\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EC15CC8-9430-4C70-9B55-C56763B7D31E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E0228B5-F43A-4ECC-AF7A-1900A226CC3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1485" yWindow="690" windowWidth="27225" windowHeight="13965" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="831" uniqueCount="484">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="835" uniqueCount="486">
   <si>
     <t>Pin Number</t>
   </si>
@@ -764,9 +764,6 @@
     <t>F1_TEMP_DIODE</t>
   </si>
   <si>
-    <t>3.08, 5.06</t>
-  </si>
-  <si>
     <t>The voltage from the LTC2997H signal conditioner connected to the temperature-sensing diode in FPGA#1.
 Scale = 4 * (1.004/1.026) millivolts per degree K.</t>
   </si>
@@ -778,9 +775,6 @@
 Scale = 4 * (1.004/1.026) millivolts per degree K.</t>
   </si>
   <si>
-    <t>3.08, 6.06</t>
-  </si>
-  <si>
     <t>V_F1_VCCAUX</t>
   </si>
   <si>
@@ -1213,16 +1207,10 @@
 lovF1_TO_MCU</t>
   </si>
   <si>
-    <t>2.10, 5.07</t>
-  </si>
-  <si>
     <t>hivF2_TO_MCU
 lovF2_TO_MCU</t>
   </si>
   <si>
-    <t>2.10, 6.07</t>
-  </si>
-  <si>
     <t>hivMCU_TO_F1
 lovMCU_TO_F1</t>
   </si>
@@ -1260,42 +1248,24 @@
     <t>MCU_LED_BLUE</t>
   </si>
   <si>
-    <t>2.10</t>
-  </si>
-  <si>
     <t>/F1_INSTALLED</t>
   </si>
   <si>
     <t>/F2_INSTALLED</t>
   </si>
   <si>
-    <t>2.10, 5.01</t>
-  </si>
-  <si>
     <t>Active-lo digital input that indicates that FPGA#1 is installed on the board. It connects to a pullup resistor and one of the GND balls on the FPGA. If the FPGA is installed, the signal is pulled low through the internal GND of the FPGA.</t>
   </si>
   <si>
-    <t>2.10, 6.01</t>
-  </si>
-  <si>
     <t>Active-lo digital input that indicates that FPGA#2 is installed on the board. It connects to a pullup resistor and one of the GND balls on the FPGA. If the FPGA is installed, the signal is pulled low through the internal GND of the FPGA.</t>
   </si>
   <si>
-    <t>2.10, 5.04</t>
-  </si>
-  <si>
     <t>/F1_CFG_DONE</t>
   </si>
   <si>
     <t>/F2_CFG_DONE</t>
   </si>
   <si>
-    <t>2.10, 6.04</t>
-  </si>
-  <si>
-    <t>2.10, 5.04, 6.04</t>
-  </si>
-  <si>
     <t>/F1_JTAG_BYPASS</t>
   </si>
   <si>
@@ -1311,12 +1281,6 @@
     <t>Active-lo digital input from FPGA#1. If the FPGA is installed, this signal will be LOW when the FPGA configuration is complete. Unfortunately, if the FPGA is not installed, it will also be LOW all the time. Therefore, it must be qualified with /F1_INSTALLED.</t>
   </si>
   <si>
-    <t>MCU_ENABLED will be HIGH when:
-a) SM_TO_CM_PWR_EN is HIGH (either from the board being operated "stand alone" or the signal driven HIGH by the service module)
-b) AND the management supply is good (V_M3V3)
-c) AND the front panel "RESET" switch is not activated.</t>
-  </si>
-  <si>
     <t>Connection to a test point on the CM circuit board. The use is currently undefined. It is recommended to configure it as an output driven LOW until a specific need is determined.</t>
   </si>
   <si>
@@ -1380,12 +1344,6 @@
     <t xml:space="preserve">This PG (power good) input will be HIGH when the LDO06c power supply for the board-wide 4.0 volt supply has been enabled and is supplying a good voltage. </t>
   </si>
   <si>
-    <t>3.02, 3.07</t>
-  </si>
-  <si>
-    <t>3.02, 3.04</t>
-  </si>
-  <si>
     <t>PG_F1_AVCC</t>
   </si>
   <si>
@@ -1405,9 +1363,6 @@
   </si>
   <si>
     <t xml:space="preserve">This PG (power good) input will be HIGH when the LT1764 power supply for FPGA#2's 1.8 volt V_F2_VCCAUX supply has been enabled and is supplying a good voltage. </t>
-  </si>
-  <si>
-    <t>3.02, 3.06</t>
   </si>
   <si>
     <t xml:space="preserve">This PG (power good) input will be HIGH when both phases of the "A" LGA80D power supply for FPGA#2's 0.9 volt V_F2_INT internal voltage have been enabled and are supplying a good voltage.  The PG signals from each phase are combined in an AND gate ahead of this input. </t>
@@ -1539,6 +1494,56 @@
 UART Module 2 transmit,
 GPIO port A bit 7,
 Timer T3</t>
+  </si>
+  <si>
+    <t>3.08, 5.05</t>
+  </si>
+  <si>
+    <t>3.08, 6.05</t>
+  </si>
+  <si>
+    <t>3.07, 3.09</t>
+  </si>
+  <si>
+    <t>2.12, 6.04</t>
+  </si>
+  <si>
+    <t>2.12, 5.04</t>
+  </si>
+  <si>
+    <t>MCU_ENABLED will be HIGH when:
+a) SM_TO_CM_PWR_EN is HIGH (either from the board being operated "stand alone" or the signal driven HIGH by the service module)
+b) AND the management supply is good (V_M3V3).</t>
+  </si>
+  <si>
+    <t>2.12, 5.08</t>
+  </si>
+  <si>
+    <t>2.12, 6.08</t>
+  </si>
+  <si>
+    <t>3.02, 3.07, 3.09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Set this output HIGH to turn on the LGA80D power supply for the board-wide 1.8 volts V_1V8 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Set this output HIGH to turn on the LGA80D power supply for the board-wide V_3V3 3.3 volt rail. This also enables the V_4V0 4.0 volt rail used by the FireFLy 12-lane transmitters that run at 25G. </t>
+  </si>
+  <si>
+    <t>2.12, 5.04, 6.04</t>
+  </si>
+  <si>
+    <t>2.12</t>
+  </si>
+  <si>
+    <t>4.01</t>
+  </si>
+  <si>
+    <t>2.12, 5.01</t>
+  </si>
+  <si>
+    <t>2.12, 6.01</t>
   </si>
 </sst>
 </file>
@@ -2026,8 +2031,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K136"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="K119" sqref="K119"/>
+    <sheetView tabSelected="1" topLeftCell="A129" workbookViewId="0">
+      <selection activeCell="H136" sqref="H136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2058,7 +2063,7 @@
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="11"/>
       <c r="B3" s="12" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -2070,7 +2075,7 @@
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="14"/>
       <c r="B5" s="12" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -2093,7 +2098,7 @@
         <v>17</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="H8" s="17" t="s">
         <v>211</v>
@@ -2220,13 +2225,13 @@
         <v>209</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="H13" s="16" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -2246,13 +2251,13 @@
         <v>208</v>
       </c>
       <c r="F14" s="4" t="s">
+        <v>261</v>
+      </c>
+      <c r="G14" s="4" t="s">
         <v>263</v>
       </c>
-      <c r="G14" s="4" t="s">
-        <v>265</v>
-      </c>
       <c r="H14" s="16" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -2272,7 +2277,7 @@
         <v>225</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="H15" s="16">
         <v>2.04</v>
@@ -2295,7 +2300,7 @@
         <v>225</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="H16" s="16">
         <v>3.08</v>
@@ -2315,10 +2320,10 @@
         <v>148</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="H17" s="16">
         <v>3.08</v>
@@ -2341,7 +2346,7 @@
         <v>56</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="H18" s="16">
         <v>3.08</v>
@@ -2364,13 +2369,13 @@
         <v>207</v>
       </c>
       <c r="F19" s="4" t="s">
+        <v>264</v>
+      </c>
+      <c r="G19" s="4" t="s">
         <v>266</v>
       </c>
-      <c r="G19" s="4" t="s">
-        <v>268</v>
-      </c>
       <c r="H19" s="16" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -2497,7 +2502,7 @@
         <v>225</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="H24" s="16">
         <v>2.04</v>
@@ -2520,7 +2525,7 @@
         <v>56</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="H25" s="16">
         <v>2.04</v>
@@ -2598,10 +2603,10 @@
         <v>237</v>
       </c>
       <c r="G28" s="13" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="H28" s="16" t="s">
-        <v>238</v>
+        <v>470</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -2621,13 +2626,13 @@
         <v>90</v>
       </c>
       <c r="F29" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="G29" s="13" t="s">
         <v>240</v>
       </c>
-      <c r="G29" s="13" t="s">
-        <v>241</v>
-      </c>
       <c r="H29" s="16" t="s">
-        <v>242</v>
+        <v>471</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -2647,13 +2652,13 @@
         <v>152</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>436</v>
+        <v>425</v>
       </c>
       <c r="H30" s="16" t="s">
-        <v>437</v>
+        <v>472</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="90" x14ac:dyDescent="0.25">
@@ -2673,13 +2678,13 @@
         <v>153</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="H31" s="16" t="s">
-        <v>408</v>
+        <v>473</v>
       </c>
     </row>
     <row r="32" spans="1:11" ht="75" x14ac:dyDescent="0.25">
@@ -2687,22 +2692,22 @@
         <v>24</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>468</v>
+        <v>454</v>
       </c>
       <c r="C32" s="5" t="s">
+        <v>314</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>314</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>466</v>
+      </c>
+      <c r="F32" s="4" t="s">
         <v>316</v>
       </c>
-      <c r="D32" s="5" t="s">
-        <v>316</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>480</v>
-      </c>
-      <c r="F32" s="4" t="s">
-        <v>318</v>
-      </c>
       <c r="G32" s="4" t="s">
-        <v>479</v>
+        <v>465</v>
       </c>
       <c r="H32" s="16">
         <v>2.0099999999999998</v>
@@ -2716,19 +2721,19 @@
         <v>112</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>481</v>
+        <v>467</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>467</v>
+        <v>453</v>
       </c>
       <c r="H33" s="16">
         <v>2.0099999999999998</v>
@@ -2751,7 +2756,7 @@
         <v>225</v>
       </c>
       <c r="G34" s="4" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="H34" s="16">
         <v>2.04</v>
@@ -2774,13 +2779,13 @@
         <v>206</v>
       </c>
       <c r="F35" s="4" t="s">
+        <v>267</v>
+      </c>
+      <c r="G35" s="4" t="s">
+        <v>268</v>
+      </c>
+      <c r="H35" s="16" t="s">
         <v>269</v>
-      </c>
-      <c r="G35" s="4" t="s">
-        <v>270</v>
-      </c>
-      <c r="H35" s="16" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -2800,7 +2805,7 @@
         <v>225</v>
       </c>
       <c r="G36" s="4" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="H36" s="16">
         <v>2.04</v>
@@ -2823,13 +2828,13 @@
         <v>154</v>
       </c>
       <c r="F37" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="G37" s="4" t="s">
         <v>272</v>
       </c>
-      <c r="G37" s="4" t="s">
-        <v>274</v>
-      </c>
       <c r="H37" s="16" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="135" x14ac:dyDescent="0.25">
@@ -2849,10 +2854,10 @@
         <v>155</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="G38" s="4" t="s">
-        <v>429</v>
+        <v>418</v>
       </c>
       <c r="H38" s="16">
         <v>2.0099999999999998</v>
@@ -2875,13 +2880,13 @@
         <v>156</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="G39" s="4" t="s">
-        <v>434</v>
+        <v>423</v>
       </c>
       <c r="H39" s="16" t="s">
-        <v>433</v>
+        <v>422</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -2901,13 +2906,13 @@
         <v>157</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="G40" s="4" t="s">
-        <v>435</v>
+        <v>424</v>
       </c>
       <c r="H40" s="16" t="s">
-        <v>433</v>
+        <v>422</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -2924,13 +2929,13 @@
         <v>7</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>473</v>
+        <v>459</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="G41" s="4" t="s">
-        <v>471</v>
+        <v>457</v>
       </c>
       <c r="H41" s="16">
         <v>2.0099999999999998</v>
@@ -2950,13 +2955,13 @@
         <v>7</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>476</v>
+        <v>462</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="G42" s="4" t="s">
-        <v>472</v>
+        <v>458</v>
       </c>
       <c r="H42" s="16">
         <v>2.0099999999999998</v>
@@ -2967,22 +2972,22 @@
         <v>35</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="C43" s="5" t="s">
         <v>37</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>477</v>
+        <v>463</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>463</v>
+        <v>449</v>
       </c>
       <c r="G43" s="4" t="s">
-        <v>465</v>
+        <v>451</v>
       </c>
       <c r="H43" s="16">
         <v>2.0099999999999998</v>
@@ -2993,22 +2998,22 @@
         <v>36</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C44" s="5" t="s">
         <v>37</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>478</v>
+        <v>464</v>
       </c>
       <c r="F44" s="4" t="s">
-        <v>464</v>
+        <v>450</v>
       </c>
       <c r="G44" s="4" t="s">
-        <v>466</v>
+        <v>452</v>
       </c>
       <c r="H44" s="16">
         <v>2.0099999999999998</v>
@@ -3019,7 +3024,7 @@
         <v>37</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C45" s="5" t="s">
         <v>9</v>
@@ -3028,13 +3033,13 @@
         <v>7</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>474</v>
+        <v>460</v>
       </c>
       <c r="F45" s="4" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="G45" s="4" t="s">
-        <v>469</v>
+        <v>455</v>
       </c>
       <c r="H45" s="16">
         <v>2.0099999999999998</v>
@@ -3045,7 +3050,7 @@
         <v>38</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C46" s="5" t="s">
         <v>6</v>
@@ -3054,13 +3059,13 @@
         <v>7</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>475</v>
+        <v>461</v>
       </c>
       <c r="F46" s="4" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="G46" s="4" t="s">
-        <v>470</v>
+        <v>456</v>
       </c>
       <c r="H46" s="16">
         <v>2.0099999999999998</v>
@@ -3083,7 +3088,7 @@
         <v>225</v>
       </c>
       <c r="G47" s="4" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="H47" s="16">
         <v>2.04</v>
@@ -3094,22 +3099,22 @@
         <v>40</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>482</v>
+        <v>468</v>
       </c>
       <c r="F48" s="4" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="G48" s="4" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="H48" s="16">
         <v>2.0099999999999998</v>
@@ -3120,22 +3125,22 @@
         <v>41</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>483</v>
+        <v>469</v>
       </c>
       <c r="F49" s="4" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="G49" s="4" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="H49" s="16">
         <v>2.0099999999999998</v>
@@ -3158,13 +3163,13 @@
         <v>158</v>
       </c>
       <c r="F50" s="4" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="G50" s="4" t="s">
-        <v>449</v>
+        <v>435</v>
       </c>
       <c r="H50" s="16" t="s">
-        <v>432</v>
+        <v>421</v>
       </c>
     </row>
     <row r="51" spans="1:8" ht="90" x14ac:dyDescent="0.25">
@@ -3184,13 +3189,13 @@
         <v>159</v>
       </c>
       <c r="F51" s="4" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="G51" s="4" t="s">
-        <v>450</v>
+        <v>436</v>
       </c>
       <c r="H51" s="16" t="s">
-        <v>432</v>
+        <v>421</v>
       </c>
     </row>
     <row r="52" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -3210,13 +3215,13 @@
         <v>160</v>
       </c>
       <c r="F52" s="4" t="s">
+        <v>426</v>
+      </c>
+      <c r="G52" s="4" t="s">
+        <v>429</v>
+      </c>
+      <c r="H52" s="16" t="s">
         <v>439</v>
-      </c>
-      <c r="G52" s="4" t="s">
-        <v>442</v>
-      </c>
-      <c r="H52" s="16" t="s">
-        <v>438</v>
       </c>
     </row>
     <row r="53" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -3236,13 +3241,13 @@
         <v>161</v>
       </c>
       <c r="F53" s="4" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="G53" s="4" t="s">
-        <v>441</v>
+        <v>428</v>
       </c>
       <c r="H53" s="16" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
     </row>
     <row r="54" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -3262,13 +3267,13 @@
         <v>205</v>
       </c>
       <c r="F54" s="4" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="G54" s="4" t="s">
-        <v>440</v>
+        <v>427</v>
       </c>
       <c r="H54" s="16" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
     </row>
     <row r="55" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -3288,7 +3293,7 @@
         <v>225</v>
       </c>
       <c r="G55" s="4" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="H55" s="16">
         <v>2.04</v>
@@ -3311,7 +3316,7 @@
         <v>56</v>
       </c>
       <c r="G56" s="4" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="H56" s="16">
         <v>2.04</v>
@@ -3328,19 +3333,19 @@
         <v>37</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="F57" s="4" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="G57" s="4" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="H57" s="16" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="58" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -3354,19 +3359,19 @@
         <v>37</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="E58" s="3" t="s">
         <v>204</v>
       </c>
       <c r="F58" s="4" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="G58" s="4" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="H58" s="16" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="59" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -3380,19 +3385,19 @@
         <v>37</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="F59" s="4" t="s">
+        <v>275</v>
+      </c>
+      <c r="G59" s="4" t="s">
         <v>277</v>
       </c>
-      <c r="G59" s="4" t="s">
-        <v>279</v>
-      </c>
       <c r="H59" s="16" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="60" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -3406,19 +3411,19 @@
         <v>37</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="E60" s="3" t="s">
         <v>203</v>
       </c>
       <c r="F60" s="4" t="s">
+        <v>276</v>
+      </c>
+      <c r="G60" s="4" t="s">
         <v>278</v>
       </c>
-      <c r="G60" s="4" t="s">
-        <v>280</v>
-      </c>
       <c r="H60" s="16" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="61" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -3432,19 +3437,19 @@
         <v>37</v>
       </c>
       <c r="D61" s="5" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="F61" s="4" t="s">
+        <v>279</v>
+      </c>
+      <c r="G61" s="4" t="s">
         <v>281</v>
       </c>
-      <c r="G61" s="4" t="s">
-        <v>283</v>
-      </c>
       <c r="H61" s="16" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="62" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -3458,19 +3463,19 @@
         <v>37</v>
       </c>
       <c r="D62" s="5" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="E62" s="3" t="s">
         <v>202</v>
       </c>
       <c r="F62" s="4" t="s">
+        <v>280</v>
+      </c>
+      <c r="G62" s="4" t="s">
         <v>282</v>
       </c>
-      <c r="G62" s="4" t="s">
-        <v>284</v>
-      </c>
       <c r="H62" s="16" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="63" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -3484,19 +3489,19 @@
         <v>37</v>
       </c>
       <c r="D63" s="5" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="E63" s="3" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="F63" s="4" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="G63" s="4" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="H63" s="16" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="64" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -3510,19 +3515,19 @@
         <v>37</v>
       </c>
       <c r="D64" s="5" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="E64" s="3" t="s">
         <v>201</v>
       </c>
       <c r="F64" s="4" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="G64" s="4" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="H64" s="16" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="65" spans="1:11" ht="90" x14ac:dyDescent="0.25">
@@ -3542,13 +3547,13 @@
         <v>162</v>
       </c>
       <c r="F65" s="4" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="G65" s="4" t="s">
-        <v>447</v>
+        <v>433</v>
       </c>
       <c r="H65" s="16" t="s">
-        <v>431</v>
+        <v>420</v>
       </c>
     </row>
     <row r="66" spans="1:11" ht="90" x14ac:dyDescent="0.25">
@@ -3568,13 +3573,13 @@
         <v>163</v>
       </c>
       <c r="F66" s="4" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="G66" s="4" t="s">
-        <v>448</v>
+        <v>434</v>
       </c>
       <c r="H66" s="16" t="s">
-        <v>431</v>
+        <v>420</v>
       </c>
     </row>
     <row r="67" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -3594,13 +3599,13 @@
         <v>164</v>
       </c>
       <c r="F67" s="4" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="G67" s="4" t="s">
-        <v>443</v>
+        <v>430</v>
       </c>
       <c r="H67" s="16" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
     </row>
     <row r="68" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -3620,13 +3625,13 @@
         <v>165</v>
       </c>
       <c r="F68" s="4" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="G68" s="4" t="s">
+        <v>431</v>
+      </c>
+      <c r="H68" s="16" t="s">
         <v>444</v>
-      </c>
-      <c r="H68" s="16" t="s">
-        <v>446</v>
       </c>
     </row>
     <row r="69" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -3646,13 +3651,13 @@
         <v>166</v>
       </c>
       <c r="F69" s="4" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="G69" s="4" t="s">
-        <v>445</v>
+        <v>432</v>
       </c>
       <c r="H69" s="16" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
     </row>
     <row r="70" spans="1:11" ht="90" x14ac:dyDescent="0.25">
@@ -3672,13 +3677,13 @@
         <v>200</v>
       </c>
       <c r="F70" s="4" t="s">
-        <v>406</v>
+        <v>398</v>
       </c>
       <c r="G70" s="4" t="s">
-        <v>414</v>
+        <v>404</v>
       </c>
       <c r="H70" s="16" t="s">
-        <v>405</v>
+        <v>474</v>
       </c>
       <c r="K70" s="4"/>
     </row>
@@ -3699,7 +3704,7 @@
         <v>225</v>
       </c>
       <c r="G71" s="4" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="H71" s="16">
         <v>2.04</v>
@@ -3752,7 +3757,7 @@
         <v>23</v>
       </c>
       <c r="G73" s="4" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="H73" s="16">
         <v>2.04</v>
@@ -3772,13 +3777,13 @@
         <v>22</v>
       </c>
       <c r="E74" s="3" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="F74" s="4" t="s">
         <v>24</v>
       </c>
       <c r="G74" s="4" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="H74" s="16">
         <v>2.04</v>
@@ -3798,13 +3803,13 @@
         <v>22</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="F75" s="4" t="s">
         <v>25</v>
       </c>
       <c r="G75" s="4" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="H75" s="16">
         <v>2.04</v>
@@ -3821,13 +3826,13 @@
         <v>54</v>
       </c>
       <c r="E76" s="3" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="F76" s="4" t="s">
         <v>225</v>
       </c>
       <c r="G76" s="4" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="H76" s="16">
         <v>2.04</v>
@@ -3850,13 +3855,13 @@
         <v>225</v>
       </c>
       <c r="G77" s="4" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="H77" s="16">
         <v>2.04</v>
       </c>
     </row>
-    <row r="78" spans="1:11" ht="120" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A78" s="10">
         <v>70</v>
       </c>
@@ -3873,10 +3878,10 @@
         <v>19</v>
       </c>
       <c r="F78" s="4" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G78" s="4" t="s">
-        <v>415</v>
+        <v>475</v>
       </c>
       <c r="H78" s="16">
         <v>2.04</v>
@@ -3899,13 +3904,13 @@
         <v>199</v>
       </c>
       <c r="F79" s="4" t="s">
-        <v>407</v>
+        <v>399</v>
       </c>
       <c r="G79" s="4" t="s">
-        <v>421</v>
+        <v>410</v>
       </c>
       <c r="H79" s="16" t="s">
-        <v>408</v>
+        <v>473</v>
       </c>
     </row>
     <row r="80" spans="1:11" ht="90" x14ac:dyDescent="0.25">
@@ -3925,13 +3930,13 @@
         <v>198</v>
       </c>
       <c r="F80" s="4" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="G80" s="4" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="H80" s="16" t="s">
-        <v>384</v>
+        <v>476</v>
       </c>
     </row>
     <row r="81" spans="1:11" ht="90" x14ac:dyDescent="0.25">
@@ -3951,13 +3956,13 @@
         <v>172</v>
       </c>
       <c r="F81" s="4" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="G81" s="4" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="H81" s="16" t="s">
-        <v>386</v>
+        <v>477</v>
       </c>
     </row>
     <row r="82" spans="1:11" ht="90" x14ac:dyDescent="0.25">
@@ -3977,13 +3982,13 @@
         <v>167</v>
       </c>
       <c r="F82" s="4" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="G82" s="4" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="H82" s="16" t="s">
-        <v>384</v>
+        <v>476</v>
       </c>
     </row>
     <row r="83" spans="1:11" ht="90" x14ac:dyDescent="0.25">
@@ -4003,13 +4008,13 @@
         <v>168</v>
       </c>
       <c r="F83" s="4" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="G83" s="4" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="H83" s="16" t="s">
-        <v>384</v>
+        <v>477</v>
       </c>
     </row>
     <row r="84" spans="1:11" ht="90" x14ac:dyDescent="0.25">
@@ -4029,16 +4034,16 @@
         <v>169</v>
       </c>
       <c r="F84" s="4" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="G84" s="4" t="s">
-        <v>430</v>
+        <v>419</v>
       </c>
       <c r="H84" s="16">
         <v>2.0099999999999998</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A85" s="8">
         <v>77</v>
       </c>
@@ -4055,10 +4060,16 @@
         <v>170</v>
       </c>
       <c r="F85" s="4" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+        <v>366</v>
+      </c>
+      <c r="G85" s="4" t="s">
+        <v>480</v>
+      </c>
+      <c r="H85" s="16" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A86" s="8">
         <v>78</v>
       </c>
@@ -4075,7 +4086,13 @@
         <v>171</v>
       </c>
       <c r="F86" s="4" t="s">
-        <v>369</v>
+        <v>367</v>
+      </c>
+      <c r="G86" s="4" t="s">
+        <v>479</v>
+      </c>
+      <c r="H86" s="16" t="s">
+        <v>422</v>
       </c>
       <c r="K86" s="4"/>
     </row>
@@ -4096,7 +4113,7 @@
         <v>225</v>
       </c>
       <c r="G87" s="4" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="H87" s="16">
         <v>2.04</v>
@@ -4119,7 +4136,7 @@
         <v>56</v>
       </c>
       <c r="G88" s="4" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="H88" s="16">
         <v>2.04</v>
@@ -4142,13 +4159,13 @@
         <v>173</v>
       </c>
       <c r="F89" s="4" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="G89" s="4" t="s">
-        <v>451</v>
+        <v>437</v>
       </c>
       <c r="H89" s="16" t="s">
-        <v>432</v>
+        <v>421</v>
       </c>
       <c r="K89" s="4"/>
     </row>
@@ -4169,13 +4186,13 @@
         <v>174</v>
       </c>
       <c r="F90" s="4" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="G90" s="4" t="s">
-        <v>456</v>
+        <v>442</v>
       </c>
       <c r="H90" s="16" t="s">
-        <v>453</v>
+        <v>439</v>
       </c>
       <c r="K90" s="4"/>
     </row>
@@ -4196,13 +4213,13 @@
         <v>175</v>
       </c>
       <c r="F91" s="4" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="G91" s="4" t="s">
-        <v>455</v>
+        <v>441</v>
       </c>
       <c r="H91" s="16" t="s">
-        <v>453</v>
+        <v>439</v>
       </c>
     </row>
     <row r="92" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -4222,13 +4239,13 @@
         <v>176</v>
       </c>
       <c r="F92" s="4" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="G92" s="4" t="s">
-        <v>454</v>
+        <v>440</v>
       </c>
       <c r="H92" s="16" t="s">
-        <v>453</v>
+        <v>439</v>
       </c>
     </row>
     <row r="93" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -4248,13 +4265,13 @@
         <v>177</v>
       </c>
       <c r="F93" s="4" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="G93" s="4" t="s">
-        <v>452</v>
+        <v>438</v>
       </c>
       <c r="H93" s="16" t="s">
-        <v>431</v>
+        <v>420</v>
       </c>
     </row>
     <row r="94" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -4274,13 +4291,13 @@
         <v>178</v>
       </c>
       <c r="F94" s="4" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="G94" s="4" t="s">
-        <v>457</v>
+        <v>443</v>
       </c>
       <c r="H94" s="16" t="s">
-        <v>458</v>
+        <v>444</v>
       </c>
     </row>
     <row r="95" spans="1:11" ht="75" x14ac:dyDescent="0.25">
@@ -4294,13 +4311,13 @@
         <v>54</v>
       </c>
       <c r="E95" s="3" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="F95" s="4" t="s">
+        <v>337</v>
+      </c>
+      <c r="G95" s="3" t="s">
         <v>339</v>
-      </c>
-      <c r="G95" s="3" t="s">
-        <v>341</v>
       </c>
       <c r="H95" s="16">
         <v>2.04</v>
@@ -4320,13 +4337,13 @@
         <v>22</v>
       </c>
       <c r="E96" s="3" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="F96" s="4" t="s">
         <v>20</v>
       </c>
       <c r="G96" s="4" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="H96" s="16">
         <v>2.04</v>
@@ -4346,13 +4363,13 @@
         <v>22</v>
       </c>
       <c r="E97" s="3" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="F97" s="4" t="s">
         <v>21</v>
       </c>
       <c r="G97" s="4" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="H97" s="16">
         <v>2.04</v>
@@ -4375,7 +4392,7 @@
         <v>225</v>
       </c>
       <c r="G98" s="4" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="H98" s="16">
         <v>2.04</v>
@@ -4392,16 +4409,16 @@
         <v>37</v>
       </c>
       <c r="D99" s="5" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="E99" s="3" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="F99" s="4" t="s">
-        <v>462</v>
+        <v>448</v>
       </c>
       <c r="G99" s="4" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="H99" s="16">
         <v>2.0099999999999998</v>
@@ -4418,16 +4435,16 @@
         <v>37</v>
       </c>
       <c r="D100" s="5" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="E100" s="3" t="s">
         <v>197</v>
       </c>
       <c r="F100" s="4" t="s">
-        <v>461</v>
+        <v>447</v>
       </c>
       <c r="G100" s="4" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="H100" s="16">
         <v>2.0099999999999998</v>
@@ -4450,13 +4467,13 @@
         <v>179</v>
       </c>
       <c r="F101" s="4" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="G101" s="4" t="s">
-        <v>459</v>
+        <v>445</v>
       </c>
       <c r="H101" s="16" t="s">
-        <v>458</v>
+        <v>444</v>
       </c>
     </row>
     <row r="102" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -4476,13 +4493,13 @@
         <v>180</v>
       </c>
       <c r="F102" s="4" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="G102" s="4" t="s">
-        <v>460</v>
+        <v>446</v>
       </c>
       <c r="H102" s="16" t="s">
-        <v>458</v>
+        <v>444</v>
       </c>
     </row>
     <row r="103" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -4490,25 +4507,25 @@
         <v>95</v>
       </c>
       <c r="B103" s="5" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C103" s="5" t="s">
         <v>37</v>
       </c>
       <c r="D103" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="E103" s="3" t="s">
         <v>301</v>
       </c>
-      <c r="E103" s="3" t="s">
-        <v>303</v>
-      </c>
       <c r="F103" s="4" t="s">
+        <v>290</v>
+      </c>
+      <c r="G103" s="4" t="s">
         <v>292</v>
       </c>
-      <c r="G103" s="4" t="s">
-        <v>294</v>
-      </c>
       <c r="H103" s="16" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="104" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -4516,25 +4533,25 @@
         <v>96</v>
       </c>
       <c r="B104" s="5" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C104" s="5" t="s">
         <v>37</v>
       </c>
       <c r="D104" s="5" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="E104" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="F104" s="4" t="s">
         <v>291</v>
       </c>
-      <c r="F104" s="4" t="s">
+      <c r="G104" s="4" t="s">
         <v>293</v>
       </c>
-      <c r="G104" s="4" t="s">
-        <v>295</v>
-      </c>
       <c r="H104" s="16" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="105" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -4554,10 +4571,10 @@
         <v>11</v>
       </c>
       <c r="F105" s="3" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="G105" s="4" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="H105" s="16">
         <v>2.0299999999999998</v>
@@ -4580,10 +4597,10 @@
         <v>181</v>
       </c>
       <c r="F106" s="3" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="G106" s="4" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="H106" s="16">
         <v>2.0299999999999998</v>
@@ -4606,10 +4623,10 @@
         <v>10</v>
       </c>
       <c r="F107" s="3" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="G107" s="4" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="H107" s="16">
         <v>2.0299999999999998</v>
@@ -4632,10 +4649,10 @@
         <v>14</v>
       </c>
       <c r="F108" s="3" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="G108" s="4" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="H108" s="16">
         <v>2.0299999999999998</v>
@@ -4658,7 +4675,7 @@
         <v>225</v>
       </c>
       <c r="G109" s="4" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="H109" s="16">
         <v>2.04</v>
@@ -4681,13 +4698,13 @@
         <v>182</v>
       </c>
       <c r="F110" s="4" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="G110" s="4" t="s">
-        <v>422</v>
+        <v>411</v>
       </c>
       <c r="H110" s="16" t="s">
-        <v>409</v>
+        <v>481</v>
       </c>
     </row>
     <row r="111" spans="1:8" ht="90" x14ac:dyDescent="0.25">
@@ -4707,13 +4724,13 @@
         <v>183</v>
       </c>
       <c r="F111" s="4" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="G111" s="4" t="s">
-        <v>417</v>
+        <v>406</v>
       </c>
       <c r="H111" s="16" t="s">
-        <v>405</v>
+        <v>474</v>
       </c>
     </row>
     <row r="112" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -4733,13 +4750,13 @@
         <v>184</v>
       </c>
       <c r="F112" s="4" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="G112" s="4" t="s">
-        <v>423</v>
+        <v>412</v>
       </c>
       <c r="H112" s="16" t="s">
-        <v>398</v>
+        <v>482</v>
       </c>
     </row>
     <row r="113" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -4759,13 +4776,13 @@
         <v>185</v>
       </c>
       <c r="F113" s="4" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="G113" s="4" t="s">
-        <v>424</v>
+        <v>413</v>
       </c>
       <c r="H113" s="16" t="s">
-        <v>398</v>
+        <v>482</v>
       </c>
     </row>
     <row r="114" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -4785,13 +4802,13 @@
         <v>186</v>
       </c>
       <c r="F114" s="4" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="G114" s="4" t="s">
-        <v>425</v>
+        <v>414</v>
       </c>
       <c r="H114" s="16" t="s">
-        <v>398</v>
+        <v>482</v>
       </c>
       <c r="K114" s="4"/>
     </row>
@@ -4812,13 +4829,13 @@
         <v>187</v>
       </c>
       <c r="F115" s="4" t="s">
-        <v>427</v>
+        <v>416</v>
       </c>
       <c r="G115" s="4" t="s">
-        <v>428</v>
+        <v>417</v>
       </c>
       <c r="H115" s="16" t="s">
-        <v>261</v>
+        <v>483</v>
       </c>
     </row>
     <row r="116" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -4838,10 +4855,10 @@
         <v>188</v>
       </c>
       <c r="F116" s="4" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="G116" s="4" t="s">
-        <v>426</v>
+        <v>415</v>
       </c>
       <c r="H116" s="16">
         <v>2.0299999999999998</v>
@@ -4864,10 +4881,10 @@
         <v>189</v>
       </c>
       <c r="F117" s="4" t="s">
-        <v>410</v>
+        <v>400</v>
       </c>
       <c r="G117" s="4" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="H117" s="16">
         <v>2.0299999999999998</v>
@@ -4890,10 +4907,10 @@
         <v>190</v>
       </c>
       <c r="F118" s="4" t="s">
-        <v>411</v>
+        <v>401</v>
       </c>
       <c r="G118" s="4" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H118" s="16">
         <v>2.0299999999999998</v>
@@ -4907,22 +4924,22 @@
         <v>118</v>
       </c>
       <c r="C119" s="5" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="D119" s="5" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E119" s="3" t="s">
         <v>191</v>
       </c>
       <c r="F119" s="4" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="G119" s="4" t="s">
-        <v>416</v>
+        <v>405</v>
       </c>
       <c r="H119" s="16" t="s">
-        <v>398</v>
+        <v>482</v>
       </c>
       <c r="K119" s="4"/>
     </row>
@@ -4934,22 +4951,22 @@
         <v>117</v>
       </c>
       <c r="C120" s="5" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="D120" s="5" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E120" s="3" t="s">
         <v>192</v>
       </c>
       <c r="F120" s="4" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="G120" s="4" t="s">
-        <v>416</v>
+        <v>405</v>
       </c>
       <c r="H120" s="16" t="s">
-        <v>398</v>
+        <v>482</v>
       </c>
       <c r="K120" s="4"/>
     </row>
@@ -4970,7 +4987,7 @@
         <v>225</v>
       </c>
       <c r="G121" s="4" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="H121" s="16">
         <v>2.04</v>
@@ -4993,7 +5010,7 @@
         <v>56</v>
       </c>
       <c r="G122" s="4" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="H122" s="16">
         <v>2.04</v>
@@ -5010,13 +5027,13 @@
         <v>54</v>
       </c>
       <c r="E123" s="3" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="F123" s="4" t="s">
+        <v>337</v>
+      </c>
+      <c r="G123" s="3" t="s">
         <v>339</v>
-      </c>
-      <c r="G123" s="3" t="s">
-        <v>341</v>
       </c>
       <c r="H123" s="16">
         <v>2.04</v>
@@ -5039,13 +5056,13 @@
         <v>193</v>
       </c>
       <c r="F124" s="4" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="G124" s="4" t="s">
-        <v>412</v>
+        <v>402</v>
       </c>
       <c r="H124" s="16" t="s">
-        <v>384</v>
+        <v>476</v>
       </c>
     </row>
     <row r="125" spans="1:11" ht="120" x14ac:dyDescent="0.25">
@@ -5065,13 +5082,13 @@
         <v>194</v>
       </c>
       <c r="F125" s="4" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="G125" s="4" t="s">
-        <v>413</v>
+        <v>403</v>
       </c>
       <c r="H125" s="16" t="s">
-        <v>386</v>
+        <v>477</v>
       </c>
     </row>
     <row r="126" spans="1:11" ht="75" x14ac:dyDescent="0.25">
@@ -5091,13 +5108,13 @@
         <v>195</v>
       </c>
       <c r="F126" s="4" t="s">
-        <v>399</v>
+        <v>394</v>
       </c>
       <c r="G126" s="4" t="s">
-        <v>402</v>
+        <v>396</v>
       </c>
       <c r="H126" s="16" t="s">
-        <v>401</v>
+        <v>484</v>
       </c>
     </row>
     <row r="127" spans="1:11" ht="75" x14ac:dyDescent="0.25">
@@ -5117,13 +5134,13 @@
         <v>196</v>
       </c>
       <c r="F127" s="4" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="G127" s="4" t="s">
-        <v>404</v>
+        <v>397</v>
       </c>
       <c r="H127" s="16" t="s">
-        <v>403</v>
+        <v>485</v>
       </c>
     </row>
     <row r="128" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -5143,10 +5160,10 @@
         <v>89</v>
       </c>
       <c r="F128" s="4" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="G128" s="4" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="H128" s="16" t="s">
         <v>221</v>
@@ -5169,10 +5186,10 @@
         <v>88</v>
       </c>
       <c r="F129" s="4" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="G129" s="4" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="H129" s="16" t="s">
         <v>221</v>
@@ -5195,7 +5212,7 @@
         <v>225</v>
       </c>
       <c r="G130" s="4" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="H130" s="16">
         <v>2.04</v>
@@ -5218,13 +5235,13 @@
         <v>87</v>
       </c>
       <c r="F131" s="4" t="s">
+        <v>252</v>
+      </c>
+      <c r="G131" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="H131" s="16" t="s">
         <v>254</v>
-      </c>
-      <c r="G131" s="4" t="s">
-        <v>255</v>
-      </c>
-      <c r="H131" s="16" t="s">
-        <v>256</v>
       </c>
     </row>
     <row r="132" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -5244,10 +5261,10 @@
         <v>86</v>
       </c>
       <c r="F132" s="4" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="G132" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="H132" s="16" t="s">
         <v>234</v>
@@ -5270,10 +5287,10 @@
         <v>85</v>
       </c>
       <c r="F133" s="4" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="G133" s="4" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="H133" s="16" t="s">
         <v>234</v>
@@ -5296,10 +5313,10 @@
         <v>84</v>
       </c>
       <c r="F134" s="4" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="G134" s="4" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="H134" s="16" t="s">
         <v>234</v>
@@ -5322,13 +5339,13 @@
         <v>83</v>
       </c>
       <c r="F135" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="G135" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="H135" s="16" t="s">
         <v>249</v>
-      </c>
-      <c r="G135" s="4" t="s">
-        <v>250</v>
-      </c>
-      <c r="H135" s="16" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="136" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -5348,10 +5365,10 @@
         <v>82</v>
       </c>
       <c r="F136" s="4" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="G136" s="4" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="H136" s="16" t="s">
         <v>227</v>

</xml_diff>